<commit_message>
20251205 TCAMP WCAMP GSCSP
</commit_message>
<xml_diff>
--- a/GUI + Reviews/New indices list.xlsx
+++ b/GUI + Reviews/New indices list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://euronext-my.sharepoint.com/personal/csonneveld_euronext_com/Documents/Documents/Projects/GUI + Reviews/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="113" documentId="8_{676A6875-F432-47B7-9717-3084B8EAD88C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4EFB3D9C-719B-4755-8B8C-A431EFCBCF93}"/>
+  <xr:revisionPtr revIDLastSave="129" documentId="8_{676A6875-F432-47B7-9717-3084B8EAD88C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FB7DFC27-4196-475C-ADEC-2DC93838EDA3}"/>
   <bookViews>
     <workbookView xWindow="-315" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{470E612D-E4A8-42B4-A972-1027153868F9}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="169">
   <si>
     <t>EEUS</t>
   </si>
@@ -526,13 +526,31 @@
   </si>
   <si>
     <t>FRESG0000249</t>
+  </si>
+  <si>
+    <t>Kelly?</t>
+  </si>
+  <si>
+    <t>Question Francesco</t>
+  </si>
+  <si>
+    <t>Index</t>
+  </si>
+  <si>
+    <t>ISIN</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Type</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -543,6 +561,13 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Verdana"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -566,12 +591,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -922,10 +948,11 @@
     <col min="4" max="4" width="12.625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="42" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7.625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.75" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="29.625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.75" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="29.625" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="20.875" hidden="1" customWidth="1"/>
     <col min="10" max="10" width="10.375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
@@ -939,7 +966,7 @@
       </c>
       <c r="F2">
         <f>COUNTIF($J$7:$J$51,E2)</f>
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
@@ -961,13 +988,25 @@
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="J6" t="s">
+      <c r="C6" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="J6" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="K6" t="s">
+      <c r="K6" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="L6" t="s">
+      <c r="L6" s="3" t="s">
         <v>107</v>
       </c>
     </row>
@@ -1753,8 +1792,11 @@
       <c r="E34" t="s">
         <v>125</v>
       </c>
+      <c r="F34" s="1" t="s">
+        <v>3</v>
+      </c>
       <c r="J34" t="s">
-        <v>115</v>
+        <v>163</v>
       </c>
       <c r="L34" s="1" t="s">
         <v>110</v>
@@ -1770,8 +1812,14 @@
       <c r="E35" t="s">
         <v>126</v>
       </c>
+      <c r="F35" s="1" t="s">
+        <v>3</v>
+      </c>
       <c r="J35" t="s">
         <v>115</v>
+      </c>
+      <c r="K35" s="1" t="s">
+        <v>105</v>
       </c>
       <c r="L35" s="1" t="s">
         <v>113</v>
@@ -1787,8 +1835,14 @@
       <c r="E36" t="s">
         <v>127</v>
       </c>
+      <c r="F36" s="1" t="s">
+        <v>3</v>
+      </c>
       <c r="J36" t="s">
         <v>115</v>
+      </c>
+      <c r="K36" s="1" t="s">
+        <v>105</v>
       </c>
       <c r="L36" s="1" t="s">
         <v>113</v>
@@ -1804,8 +1858,14 @@
       <c r="E37" t="s">
         <v>128</v>
       </c>
+      <c r="F37" s="1" t="s">
+        <v>3</v>
+      </c>
       <c r="J37" t="s">
         <v>115</v>
+      </c>
+      <c r="K37" s="1" t="s">
+        <v>105</v>
       </c>
       <c r="L37" s="1" t="s">
         <v>113</v>
@@ -1821,6 +1881,9 @@
       <c r="E38" t="s">
         <v>129</v>
       </c>
+      <c r="F38" s="1" t="s">
+        <v>3</v>
+      </c>
       <c r="J38" t="s">
         <v>106</v>
       </c>
@@ -1841,6 +1904,9 @@
       <c r="E39" t="s">
         <v>130</v>
       </c>
+      <c r="F39" s="1" t="s">
+        <v>3</v>
+      </c>
       <c r="J39" t="s">
         <v>106</v>
       </c>
@@ -1858,6 +1924,9 @@
       <c r="E40" t="s">
         <v>131</v>
       </c>
+      <c r="F40" s="1" t="s">
+        <v>3</v>
+      </c>
       <c r="J40" t="s">
         <v>106</v>
       </c>
@@ -1875,6 +1944,9 @@
       <c r="E41" t="s">
         <v>132</v>
       </c>
+      <c r="F41" s="1" t="s">
+        <v>3</v>
+      </c>
       <c r="J41" t="s">
         <v>106</v>
       </c>
@@ -1892,6 +1964,9 @@
       <c r="E42" t="s">
         <v>133</v>
       </c>
+      <c r="F42" s="1" t="s">
+        <v>3</v>
+      </c>
       <c r="J42" t="s">
         <v>106</v>
       </c>
@@ -1909,6 +1984,9 @@
       <c r="E43" t="s">
         <v>134</v>
       </c>
+      <c r="F43" s="1" t="s">
+        <v>3</v>
+      </c>
       <c r="J43" t="s">
         <v>106</v>
       </c>
@@ -1929,6 +2007,9 @@
       <c r="E44" t="s">
         <v>135</v>
       </c>
+      <c r="F44" s="1" t="s">
+        <v>3</v>
+      </c>
       <c r="J44" t="s">
         <v>106</v>
       </c>
@@ -1946,6 +2027,9 @@
       <c r="E45" t="s">
         <v>136</v>
       </c>
+      <c r="F45" s="1" t="s">
+        <v>3</v>
+      </c>
       <c r="J45" t="s">
         <v>115</v>
       </c>
@@ -1966,8 +2050,14 @@
       <c r="E46" t="s">
         <v>137</v>
       </c>
+      <c r="F46" s="1" t="s">
+        <v>3</v>
+      </c>
       <c r="J46" t="s">
         <v>115</v>
+      </c>
+      <c r="K46" t="s">
+        <v>164</v>
       </c>
       <c r="L46" s="2" t="s">
         <v>112</v>
@@ -1983,6 +2073,9 @@
       <c r="E47" t="s">
         <v>138</v>
       </c>
+      <c r="F47" s="1" t="s">
+        <v>3</v>
+      </c>
       <c r="J47" t="s">
         <v>115</v>
       </c>
@@ -2000,6 +2093,9 @@
       <c r="E48" t="s">
         <v>139</v>
       </c>
+      <c r="F48" s="1" t="s">
+        <v>3</v>
+      </c>
       <c r="J48" t="s">
         <v>115</v>
       </c>
@@ -2017,6 +2113,9 @@
       <c r="E49" t="s">
         <v>140</v>
       </c>
+      <c r="F49" s="1" t="s">
+        <v>3</v>
+      </c>
       <c r="J49" t="s">
         <v>115</v>
       </c>
@@ -2034,6 +2133,9 @@
       <c r="E50" t="s">
         <v>141</v>
       </c>
+      <c r="F50" s="1" t="s">
+        <v>3</v>
+      </c>
       <c r="J50" t="s">
         <v>115</v>
       </c>
@@ -2050,6 +2152,9 @@
       </c>
       <c r="E51" t="s">
         <v>142</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>3</v>
       </c>
       <c r="J51" t="s">
         <v>115</v>
@@ -2071,7 +2176,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAB023AF-1979-4B95-B964-82DE009328D3}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B40" sqref="B40"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData/>

</xml_diff>

<commit_message>
20251209 EDWP + EDWPT updated for new rule CUSIP
</commit_message>
<xml_diff>
--- a/GUI + Reviews/New indices list.xlsx
+++ b/GUI + Reviews/New indices list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://euronext-my.sharepoint.com/personal/csonneveld_euronext_com/Documents/Documents/Projects/GUI + Reviews/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="141" documentId="8_{676A6875-F432-47B7-9717-3084B8EAD88C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CD114B5B-7876-4572-BABD-220F2AD6B434}"/>
+  <xr:revisionPtr revIDLastSave="142" documentId="8_{676A6875-F432-47B7-9717-3084B8EAD88C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6A1EFD46-370C-4B8E-BD38-DE757C4714F6}"/>
   <bookViews>
     <workbookView xWindow="-29115" yWindow="-16005" windowWidth="29040" windowHeight="15720" xr2:uid="{470E612D-E4A8-42B4-A972-1027153868F9}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="174">
   <si>
     <t>EEUS</t>
   </si>
@@ -556,6 +556,9 @@
   </si>
   <si>
     <t>SBF80</t>
+  </si>
+  <si>
+    <t>Same EZCLA etc</t>
   </si>
 </sst>
 </file>
@@ -983,7 +986,7 @@
   <dimension ref="A1:L56"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A35" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K56" sqref="K56"/>
+      <selection activeCell="L55" sqref="L55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2236,6 +2239,9 @@
       </c>
       <c r="J54" t="s">
         <v>115</v>
+      </c>
+      <c r="L54" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="55" spans="3:12" ht="14.25" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
20251220 FCLSP + JPCLA + JPCLE
</commit_message>
<xml_diff>
--- a/GUI + Reviews/New indices list.xlsx
+++ b/GUI + Reviews/New indices list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://euronext-my.sharepoint.com/personal/csonneveld_euronext_com/Documents/Documents/Projects/GUI + Reviews/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="236" documentId="8_{676A6875-F432-47B7-9717-3084B8EAD88C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{15E82FD2-8FBD-4496-BB50-BEA3D5688A85}"/>
+  <xr:revisionPtr revIDLastSave="256" documentId="8_{676A6875-F432-47B7-9717-3084B8EAD88C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0317F1D1-5316-4B0F-956C-06DAFC5B0FE8}"/>
   <bookViews>
-    <workbookView xWindow="-29115" yWindow="-16005" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{470E612D-E4A8-42B4-A972-1027153868F9}"/>
+    <workbookView xWindow="-29115" yWindow="-16005" windowWidth="29040" windowHeight="15720" xr2:uid="{470E612D-E4A8-42B4-A972-1027153868F9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1320" uniqueCount="350">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1326" uniqueCount="349">
   <si>
     <t>EEUS</t>
   </si>
@@ -1081,16 +1081,13 @@
     <t>Y</t>
   </si>
   <si>
-    <t>Roberto</t>
-  </si>
-  <si>
     <t>Macro</t>
   </si>
   <si>
-    <t>Macro + Capping?</t>
-  </si>
-  <si>
-    <t>Check</t>
+    <t>Fix Stellantis bug</t>
+  </si>
+  <si>
+    <t>Macro + Capping? + NACE</t>
   </si>
 </sst>
 </file>
@@ -1100,7 +1097,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yy;@"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -1660,11 +1657,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D383C28F-91C6-4BF4-880E-D92A2D8D2AE9}">
   <dimension ref="A1:L56"/>
   <sheetViews>
-    <sheetView topLeftCell="A27" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K54" sqref="K54"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="6.625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.625" bestFit="1" customWidth="1"/>
@@ -1677,12 +1674,12 @@
     <col min="11" max="11" width="17.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="E2" t="s">
         <v>115</v>
       </c>
@@ -1691,7 +1688,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="E3" t="s">
         <v>114</v>
       </c>
@@ -1700,7 +1697,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="E4" t="s">
         <v>106</v>
       </c>
@@ -1709,7 +1706,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:12">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="C6" s="3" t="s">
         <v>164</v>
       </c>
@@ -1732,7 +1729,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="15">
+    <row r="7" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="C7" s="1" t="s">
         <v>81</v>
       </c>
@@ -1752,7 +1749,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="15">
+    <row r="8" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="C8" s="1" t="s">
         <v>82</v>
       </c>
@@ -1772,7 +1769,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="15">
+    <row r="9" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="C9" s="1" t="s">
         <v>0</v>
       </c>
@@ -1801,7 +1798,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="15">
+    <row r="10" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="C10" s="1" t="s">
         <v>6</v>
       </c>
@@ -1830,7 +1827,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="15">
+    <row r="11" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="C11" s="1" t="s">
         <v>9</v>
       </c>
@@ -1859,7 +1856,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="15">
+    <row r="12" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="C12" s="1" t="s">
         <v>12</v>
       </c>
@@ -1888,7 +1885,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="15">
+    <row r="13" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="C13" s="1" t="s">
         <v>15</v>
       </c>
@@ -1917,7 +1914,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="15">
+    <row r="14" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="C14" s="1" t="s">
         <v>18</v>
       </c>
@@ -1946,7 +1943,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="15">
+    <row r="15" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="C15" s="1" t="s">
         <v>21</v>
       </c>
@@ -1975,7 +1972,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="15">
+    <row r="16" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="C16" s="1" t="s">
         <v>25</v>
       </c>
@@ -2004,7 +2001,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="17" spans="3:12" ht="15">
+    <row r="17" spans="3:12" ht="15" x14ac:dyDescent="0.2">
       <c r="C17" s="1" t="s">
         <v>29</v>
       </c>
@@ -2033,7 +2030,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="18" spans="3:12" ht="15">
+    <row r="18" spans="3:12" ht="15" x14ac:dyDescent="0.2">
       <c r="C18" s="1" t="s">
         <v>32</v>
       </c>
@@ -2062,7 +2059,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="19" spans="3:12" ht="15">
+    <row r="19" spans="3:12" ht="15" x14ac:dyDescent="0.2">
       <c r="C19" s="1" t="s">
         <v>35</v>
       </c>
@@ -2091,7 +2088,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="20" spans="3:12" ht="15">
+    <row r="20" spans="3:12" ht="15" x14ac:dyDescent="0.2">
       <c r="C20" s="1" t="s">
         <v>38</v>
       </c>
@@ -2120,7 +2117,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="21" spans="3:12" ht="15">
+    <row r="21" spans="3:12" ht="15" x14ac:dyDescent="0.2">
       <c r="C21" s="1" t="s">
         <v>41</v>
       </c>
@@ -2148,7 +2145,7 @@
       <c r="K21" s="1"/>
       <c r="L21" s="1"/>
     </row>
-    <row r="22" spans="3:12" ht="15">
+    <row r="22" spans="3:12" ht="15" x14ac:dyDescent="0.2">
       <c r="C22" s="1" t="s">
         <v>44</v>
       </c>
@@ -2178,7 +2175,7 @@
       </c>
       <c r="L22" s="1"/>
     </row>
-    <row r="23" spans="3:12" ht="15">
+    <row r="23" spans="3:12" ht="15" x14ac:dyDescent="0.2">
       <c r="C23" s="1" t="s">
         <v>47</v>
       </c>
@@ -2206,7 +2203,7 @@
       <c r="K23" s="1"/>
       <c r="L23" s="1"/>
     </row>
-    <row r="24" spans="3:12" ht="15">
+    <row r="24" spans="3:12" ht="15" x14ac:dyDescent="0.2">
       <c r="C24" s="1" t="s">
         <v>51</v>
       </c>
@@ -2236,7 +2233,7 @@
       </c>
       <c r="L24" s="1"/>
     </row>
-    <row r="25" spans="3:12" ht="15">
+    <row r="25" spans="3:12" ht="15" x14ac:dyDescent="0.2">
       <c r="C25" s="1" t="s">
         <v>54</v>
       </c>
@@ -2264,7 +2261,7 @@
       <c r="K25" s="1"/>
       <c r="L25" s="1"/>
     </row>
-    <row r="26" spans="3:12" ht="15">
+    <row r="26" spans="3:12" ht="15" x14ac:dyDescent="0.2">
       <c r="C26" s="1" t="s">
         <v>57</v>
       </c>
@@ -2294,7 +2291,7 @@
       </c>
       <c r="L26" s="1"/>
     </row>
-    <row r="27" spans="3:12" ht="15">
+    <row r="27" spans="3:12" ht="15" x14ac:dyDescent="0.2">
       <c r="C27" s="1" t="s">
         <v>60</v>
       </c>
@@ -2324,7 +2321,7 @@
       </c>
       <c r="L27" s="1"/>
     </row>
-    <row r="28" spans="3:12" ht="15">
+    <row r="28" spans="3:12" ht="15" x14ac:dyDescent="0.2">
       <c r="C28" s="1" t="s">
         <v>63</v>
       </c>
@@ -2354,7 +2351,7 @@
       </c>
       <c r="L28" s="1"/>
     </row>
-    <row r="29" spans="3:12" ht="15">
+    <row r="29" spans="3:12" ht="15" x14ac:dyDescent="0.2">
       <c r="C29" s="1" t="s">
         <v>66</v>
       </c>
@@ -2384,7 +2381,7 @@
       </c>
       <c r="L29" s="1"/>
     </row>
-    <row r="30" spans="3:12" ht="15">
+    <row r="30" spans="3:12" ht="15" x14ac:dyDescent="0.2">
       <c r="C30" s="1" t="s">
         <v>69</v>
       </c>
@@ -2414,7 +2411,7 @@
       </c>
       <c r="L30" s="1"/>
     </row>
-    <row r="31" spans="3:12" ht="15">
+    <row r="31" spans="3:12" ht="15" x14ac:dyDescent="0.2">
       <c r="C31" s="1" t="s">
         <v>72</v>
       </c>
@@ -2444,7 +2441,7 @@
       </c>
       <c r="L31" s="1"/>
     </row>
-    <row r="32" spans="3:12" ht="15">
+    <row r="32" spans="3:12" ht="15" x14ac:dyDescent="0.2">
       <c r="C32" s="1" t="s">
         <v>75</v>
       </c>
@@ -2474,7 +2471,7 @@
       </c>
       <c r="L32" s="1"/>
     </row>
-    <row r="33" spans="3:12" ht="15">
+    <row r="33" spans="3:12" ht="15" x14ac:dyDescent="0.2">
       <c r="C33" s="1" t="s">
         <v>78</v>
       </c>
@@ -2504,7 +2501,7 @@
       </c>
       <c r="L33" s="1"/>
     </row>
-    <row r="34" spans="3:12" ht="15">
+    <row r="34" spans="3:12" ht="15" x14ac:dyDescent="0.2">
       <c r="C34" s="1" t="s">
         <v>83</v>
       </c>
@@ -2524,7 +2521,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="35" spans="3:12" ht="15">
+    <row r="35" spans="3:12" ht="15" x14ac:dyDescent="0.2">
       <c r="C35" s="1" t="s">
         <v>84</v>
       </c>
@@ -2547,7 +2544,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="36" spans="3:12" ht="15">
+    <row r="36" spans="3:12" ht="15" x14ac:dyDescent="0.2">
       <c r="C36" s="1" t="s">
         <v>85</v>
       </c>
@@ -2570,7 +2567,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="37" spans="3:12" ht="15">
+    <row r="37" spans="3:12" ht="15" x14ac:dyDescent="0.2">
       <c r="C37" s="1" t="s">
         <v>86</v>
       </c>
@@ -2593,7 +2590,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="38" spans="3:12" ht="15">
+    <row r="38" spans="3:12" ht="15" x14ac:dyDescent="0.2">
       <c r="C38" s="1" t="s">
         <v>87</v>
       </c>
@@ -2616,7 +2613,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="39" spans="3:12" ht="15">
+    <row r="39" spans="3:12" ht="15" x14ac:dyDescent="0.2">
       <c r="C39" s="1" t="s">
         <v>88</v>
       </c>
@@ -2636,7 +2633,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="40" spans="3:12" ht="15">
+    <row r="40" spans="3:12" ht="15" x14ac:dyDescent="0.2">
       <c r="C40" s="1" t="s">
         <v>89</v>
       </c>
@@ -2656,7 +2653,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="41" spans="3:12" ht="15">
+    <row r="41" spans="3:12" ht="15" x14ac:dyDescent="0.2">
       <c r="C41" s="1" t="s">
         <v>90</v>
       </c>
@@ -2676,7 +2673,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="42" spans="3:12" ht="15">
+    <row r="42" spans="3:12" ht="15" x14ac:dyDescent="0.2">
       <c r="C42" s="1" t="s">
         <v>91</v>
       </c>
@@ -2696,7 +2693,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="43" spans="3:12" ht="15">
+    <row r="43" spans="3:12" ht="15" x14ac:dyDescent="0.2">
       <c r="C43" s="1" t="s">
         <v>92</v>
       </c>
@@ -2719,7 +2716,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="44" spans="3:12" ht="15">
+    <row r="44" spans="3:12" ht="15" x14ac:dyDescent="0.2">
       <c r="C44" s="1" t="s">
         <v>93</v>
       </c>
@@ -2739,7 +2736,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="45" spans="3:12" ht="15">
+    <row r="45" spans="3:12" ht="15" x14ac:dyDescent="0.2">
       <c r="C45" s="1" t="s">
         <v>94</v>
       </c>
@@ -2762,7 +2759,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="46" spans="3:12" ht="15">
+    <row r="46" spans="3:12" ht="15" x14ac:dyDescent="0.2">
       <c r="C46" s="1" t="s">
         <v>95</v>
       </c>
@@ -2785,7 +2782,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="47" spans="3:12" ht="15">
+    <row r="47" spans="3:12" ht="15" x14ac:dyDescent="0.2">
       <c r="C47" s="1" t="s">
         <v>96</v>
       </c>
@@ -2808,7 +2805,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="48" spans="3:12" ht="15">
+    <row r="48" spans="3:12" ht="15" x14ac:dyDescent="0.2">
       <c r="C48" s="1" t="s">
         <v>97</v>
       </c>
@@ -2831,7 +2828,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="49" spans="3:12" ht="15">
+    <row r="49" spans="3:12" ht="15" x14ac:dyDescent="0.2">
       <c r="C49" s="1" t="s">
         <v>98</v>
       </c>
@@ -2854,7 +2851,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="50" spans="3:12" ht="15">
+    <row r="50" spans="3:12" ht="15" x14ac:dyDescent="0.2">
       <c r="C50" s="1" t="s">
         <v>99</v>
       </c>
@@ -2877,7 +2874,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="51" spans="3:12" ht="15">
+    <row r="51" spans="3:12" ht="15" x14ac:dyDescent="0.2">
       <c r="C51" s="1" t="s">
         <v>100</v>
       </c>
@@ -2900,7 +2897,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="53" spans="3:12" ht="15">
+    <row r="53" spans="3:12" ht="15" x14ac:dyDescent="0.2">
       <c r="C53" s="1" t="s">
         <v>169</v>
       </c>
@@ -2911,7 +2908,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="54" spans="3:12" ht="15">
+    <row r="54" spans="3:12" ht="15" x14ac:dyDescent="0.2">
       <c r="C54" s="1" t="s">
         <v>170</v>
       </c>
@@ -2922,7 +2919,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="55" spans="3:12" ht="14.25">
+    <row r="55" spans="3:12" ht="14.25" x14ac:dyDescent="0.2">
       <c r="C55" s="4" t="s">
         <v>171</v>
       </c>
@@ -2930,7 +2927,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="56" spans="3:12" ht="15">
+    <row r="56" spans="3:12" ht="15" x14ac:dyDescent="0.2">
       <c r="C56" s="5" t="s">
         <v>172</v>
       </c>
@@ -2958,13 +2955,13 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F368BCE2-BE99-4B2E-A17A-1E5FAB5A74C3}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:O97"/>
+  <dimension ref="A1:O105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D101" sqref="D101:D107"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23.25" bestFit="1" customWidth="1"/>
@@ -2981,7 +2978,7 @@
     <col min="15" max="15" width="125.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="15">
+    <row r="1" spans="1:15" ht="15" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
         <v>174</v>
       </c>
@@ -3028,7 +3025,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="15" hidden="1">
+    <row r="2" spans="1:15" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2" s="8">
         <v>45982</v>
       </c>
@@ -3075,7 +3072,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="15" hidden="1">
+    <row r="3" spans="1:15" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8">
         <v>45982</v>
       </c>
@@ -3122,7 +3119,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="4" spans="1:15" ht="15" hidden="1">
+    <row r="4" spans="1:15" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A4" s="8">
         <v>45982</v>
       </c>
@@ -3169,7 +3166,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="15" hidden="1">
+    <row r="5" spans="1:15" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A5" s="8">
         <v>45982</v>
       </c>
@@ -3216,7 +3213,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="15" hidden="1">
+    <row r="6" spans="1:15" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A6" s="8">
         <v>45982</v>
       </c>
@@ -3263,7 +3260,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="7" spans="1:15" ht="15">
+    <row r="7" spans="1:15" ht="15" x14ac:dyDescent="0.2">
       <c r="A7" s="8">
         <v>45982</v>
       </c>
@@ -3308,7 +3305,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="8" spans="1:15" ht="15" hidden="1">
+    <row r="8" spans="1:15" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A8" s="8">
         <v>45982</v>
       </c>
@@ -3355,7 +3352,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="9" spans="1:15" ht="15" hidden="1">
+    <row r="9" spans="1:15" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A9" s="8">
         <v>45982</v>
       </c>
@@ -3402,7 +3399,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="10" spans="1:15" ht="15">
+    <row r="10" spans="1:15" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A10" s="8">
         <v>45982</v>
       </c>
@@ -3424,7 +3421,9 @@
       <c r="G10" s="9" t="s">
         <v>268</v>
       </c>
-      <c r="H10" s="9"/>
+      <c r="H10" s="9" t="s">
+        <v>345</v>
+      </c>
       <c r="I10" s="9" t="s">
         <v>269</v>
       </c>
@@ -3447,7 +3446,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="11" spans="1:15" ht="15" hidden="1">
+    <row r="11" spans="1:15" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A11" s="8">
         <v>45982</v>
       </c>
@@ -3494,7 +3493,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="12" spans="1:15" ht="15" hidden="1">
+    <row r="12" spans="1:15" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A12" s="8">
         <v>45982</v>
       </c>
@@ -3541,7 +3540,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="13" spans="1:15" ht="15" hidden="1">
+    <row r="13" spans="1:15" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A13" s="8">
         <v>45982</v>
       </c>
@@ -3588,7 +3587,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="14" spans="1:15" ht="15" hidden="1">
+    <row r="14" spans="1:15" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A14" s="8">
         <v>45982</v>
       </c>
@@ -3635,7 +3634,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="15" spans="1:15" ht="15" hidden="1">
+    <row r="15" spans="1:15" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A15" s="8">
         <v>45982</v>
       </c>
@@ -3682,7 +3681,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="16" spans="1:15" ht="15" hidden="1">
+    <row r="16" spans="1:15" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A16" s="8">
         <v>45982</v>
       </c>
@@ -3729,7 +3728,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="17" spans="1:15" ht="15" hidden="1">
+    <row r="17" spans="1:15" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A17" s="8">
         <v>45982</v>
       </c>
@@ -3776,7 +3775,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="18" spans="1:15" ht="15" hidden="1">
+    <row r="18" spans="1:15" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A18" s="8">
         <v>45982</v>
       </c>
@@ -3823,7 +3822,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="19" spans="1:15" ht="15" hidden="1">
+    <row r="19" spans="1:15" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A19" s="8">
         <v>45982</v>
       </c>
@@ -3870,7 +3869,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="20" spans="1:15" ht="15" hidden="1">
+    <row r="20" spans="1:15" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A20" s="8">
         <v>45982</v>
       </c>
@@ -3917,7 +3916,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="21" spans="1:15" ht="15" hidden="1">
+    <row r="21" spans="1:15" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A21" s="8">
         <v>45982</v>
       </c>
@@ -3964,7 +3963,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="22" spans="1:15" ht="15" hidden="1">
+    <row r="22" spans="1:15" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A22" s="8">
         <v>45982</v>
       </c>
@@ -4011,7 +4010,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="23" spans="1:15" ht="15" hidden="1">
+    <row r="23" spans="1:15" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A23" s="8">
         <v>45982</v>
       </c>
@@ -4058,7 +4057,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="24" spans="1:15" ht="15">
+    <row r="24" spans="1:15" ht="15" x14ac:dyDescent="0.2">
       <c r="A24" s="8">
         <v>45982</v>
       </c>
@@ -4080,7 +4079,9 @@
       <c r="G24" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="H24" s="9"/>
+      <c r="H24" s="9" t="s">
+        <v>108</v>
+      </c>
       <c r="I24" s="9" t="s">
         <v>49</v>
       </c>
@@ -4103,7 +4104,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="25" spans="1:15" ht="15" hidden="1">
+    <row r="25" spans="1:15" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A25" s="8">
         <v>45982</v>
       </c>
@@ -4150,7 +4151,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="26" spans="1:15" ht="15" hidden="1">
+    <row r="26" spans="1:15" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A26" s="8">
         <v>45982</v>
       </c>
@@ -4197,7 +4198,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="27" spans="1:15" ht="15" hidden="1">
+    <row r="27" spans="1:15" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A27" s="8">
         <v>45982</v>
       </c>
@@ -4244,7 +4245,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="28" spans="1:15" ht="15" hidden="1">
+    <row r="28" spans="1:15" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A28" s="8">
         <v>45982</v>
       </c>
@@ -4291,7 +4292,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="29" spans="1:15" ht="15" hidden="1">
+    <row r="29" spans="1:15" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A29" s="8">
         <v>45982</v>
       </c>
@@ -4338,7 +4339,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="30" spans="1:15" ht="15">
+    <row r="30" spans="1:15" ht="15" x14ac:dyDescent="0.2">
       <c r="A30" s="14">
         <v>45982</v>
       </c>
@@ -4360,7 +4361,9 @@
       <c r="G30" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="H30" s="15"/>
+      <c r="H30" s="9" t="s">
+        <v>108</v>
+      </c>
       <c r="I30" s="15" t="s">
         <v>341</v>
       </c>
@@ -4383,7 +4386,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="31" spans="1:15" ht="15" hidden="1">
+    <row r="31" spans="1:15" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A31" s="8">
         <v>45982</v>
       </c>
@@ -4430,7 +4433,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="32" spans="1:15" ht="15" hidden="1">
+    <row r="32" spans="1:15" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A32" s="14">
         <v>45982</v>
       </c>
@@ -4477,7 +4480,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="33" spans="1:15" ht="15" hidden="1">
+    <row r="33" spans="1:15" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A33" s="8">
         <v>45982</v>
       </c>
@@ -4524,7 +4527,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="34" spans="1:15" ht="15" hidden="1">
+    <row r="34" spans="1:15" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A34" s="8">
         <v>45982</v>
       </c>
@@ -4571,7 +4574,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="35" spans="1:15" ht="15" hidden="1">
+    <row r="35" spans="1:15" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A35" s="14">
         <v>45982</v>
       </c>
@@ -4618,7 +4621,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="36" spans="1:15" ht="15" hidden="1">
+    <row r="36" spans="1:15" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A36" s="8">
         <v>45982</v>
       </c>
@@ -4665,7 +4668,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="37" spans="1:15" ht="15" hidden="1">
+    <row r="37" spans="1:15" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A37" s="8">
         <v>45982</v>
       </c>
@@ -4712,7 +4715,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="38" spans="1:15" ht="15" hidden="1">
+    <row r="38" spans="1:15" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A38" s="8">
         <v>45982</v>
       </c>
@@ -4759,7 +4762,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="39" spans="1:15" ht="15">
+    <row r="39" spans="1:15" ht="15" x14ac:dyDescent="0.2">
       <c r="A39" s="8">
         <v>45982</v>
       </c>
@@ -4781,7 +4784,9 @@
       <c r="G39" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="H39" s="9"/>
+      <c r="H39" s="9" t="s">
+        <v>108</v>
+      </c>
       <c r="I39" s="9" t="s">
         <v>43</v>
       </c>
@@ -4804,7 +4809,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="40" spans="1:15" ht="15" hidden="1">
+    <row r="40" spans="1:15" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A40" s="8">
         <v>45982</v>
       </c>
@@ -4851,7 +4856,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="41" spans="1:15" ht="15">
+    <row r="41" spans="1:15" ht="15" x14ac:dyDescent="0.2">
       <c r="A41" s="8">
         <v>45982</v>
       </c>
@@ -4873,7 +4878,9 @@
       <c r="G41" s="9" t="s">
         <v>311</v>
       </c>
-      <c r="H41" s="9"/>
+      <c r="H41" s="9" t="s">
+        <v>108</v>
+      </c>
       <c r="I41" s="9" t="s">
         <v>312</v>
       </c>
@@ -4896,7 +4903,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="42" spans="1:15" ht="15" hidden="1">
+    <row r="42" spans="1:15" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A42" s="8">
         <v>45982</v>
       </c>
@@ -4943,7 +4950,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="43" spans="1:15" ht="15" hidden="1">
+    <row r="43" spans="1:15" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A43" s="8">
         <v>45982</v>
       </c>
@@ -4990,7 +4997,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="44" spans="1:15" ht="15" hidden="1">
+    <row r="44" spans="1:15" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A44" s="8">
         <v>45982</v>
       </c>
@@ -5037,7 +5044,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="45" spans="1:15" ht="15" hidden="1">
+    <row r="45" spans="1:15" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A45" s="8">
         <v>45982</v>
       </c>
@@ -5084,7 +5091,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="46" spans="1:15" ht="15" hidden="1">
+    <row r="46" spans="1:15" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A46" s="8">
         <v>45982</v>
       </c>
@@ -5131,7 +5138,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="47" spans="1:15" ht="15" hidden="1">
+    <row r="47" spans="1:15" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A47" s="8">
         <v>45982</v>
       </c>
@@ -5178,7 +5185,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="48" spans="1:15" ht="15">
+    <row r="48" spans="1:15" ht="15" x14ac:dyDescent="0.2">
       <c r="A48" s="14">
         <v>45982</v>
       </c>
@@ -5200,7 +5207,9 @@
       <c r="G48" s="15" t="s">
         <v>342</v>
       </c>
-      <c r="H48" s="15"/>
+      <c r="H48" s="9" t="s">
+        <v>108</v>
+      </c>
       <c r="I48" s="15" t="s">
         <v>343</v>
       </c>
@@ -5223,7 +5232,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="49" spans="1:15" ht="15" hidden="1">
+    <row r="49" spans="1:15" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A49" s="8">
         <v>45982</v>
       </c>
@@ -5270,7 +5279,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="50" spans="1:15" ht="15" hidden="1">
+    <row r="50" spans="1:15" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A50" s="8">
         <v>45982</v>
       </c>
@@ -5317,7 +5326,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="51" spans="1:15" ht="15" hidden="1">
+    <row r="51" spans="1:15" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A51" s="8">
         <v>45982</v>
       </c>
@@ -5364,7 +5373,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="52" spans="1:15" ht="15" hidden="1">
+    <row r="52" spans="1:15" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A52" s="8">
         <v>45982</v>
       </c>
@@ -5411,7 +5420,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="53" spans="1:15" ht="15" hidden="1">
+    <row r="53" spans="1:15" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A53" s="8">
         <v>45982</v>
       </c>
@@ -5458,7 +5467,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="54" spans="1:15" ht="15" hidden="1">
+    <row r="54" spans="1:15" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A54" s="8">
         <v>45982</v>
       </c>
@@ -5505,7 +5514,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="55" spans="1:15" ht="15" hidden="1">
+    <row r="55" spans="1:15" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A55" s="8">
         <v>45982</v>
       </c>
@@ -5552,7 +5561,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="56" spans="1:15" ht="15" hidden="1">
+    <row r="56" spans="1:15" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A56" s="8">
         <v>45982</v>
       </c>
@@ -5599,7 +5608,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="57" spans="1:15" ht="15" hidden="1">
+    <row r="57" spans="1:15" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A57" s="14">
         <v>45982</v>
       </c>
@@ -5646,7 +5655,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="58" spans="1:15" ht="15" hidden="1">
+    <row r="58" spans="1:15" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A58" s="8">
         <v>45982</v>
       </c>
@@ -5693,7 +5702,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="59" spans="1:15" ht="15" hidden="1">
+    <row r="59" spans="1:15" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A59" s="8">
         <v>45982</v>
       </c>
@@ -5740,7 +5749,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="60" spans="1:15" ht="15" hidden="1">
+    <row r="60" spans="1:15" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A60" s="14">
         <v>45982</v>
       </c>
@@ -5787,7 +5796,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="61" spans="1:15" ht="15" hidden="1">
+    <row r="61" spans="1:15" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A61" s="8">
         <v>45982</v>
       </c>
@@ -5834,7 +5843,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="62" spans="1:15" ht="15" hidden="1">
+    <row r="62" spans="1:15" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A62" s="8">
         <v>45982</v>
       </c>
@@ -5881,7 +5890,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="63" spans="1:15" ht="15" hidden="1">
+    <row r="63" spans="1:15" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A63" s="8">
         <v>45982</v>
       </c>
@@ -5928,7 +5937,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="64" spans="1:15" ht="15" hidden="1">
+    <row r="64" spans="1:15" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A64" s="14">
         <v>45982</v>
       </c>
@@ -5975,7 +5984,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="65" spans="1:15" ht="15" hidden="1">
+    <row r="65" spans="1:15" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A65" s="14">
         <v>45982</v>
       </c>
@@ -6022,7 +6031,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="66" spans="1:15" ht="15" hidden="1">
+    <row r="66" spans="1:15" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A66" s="8">
         <v>45982</v>
       </c>
@@ -6069,7 +6078,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="67" spans="1:15" ht="15" hidden="1">
+    <row r="67" spans="1:15" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A67" s="8">
         <v>45982</v>
       </c>
@@ -6116,7 +6125,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="68" spans="1:15" ht="15" hidden="1">
+    <row r="68" spans="1:15" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A68" s="8">
         <v>45982</v>
       </c>
@@ -6163,7 +6172,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="69" spans="1:15" ht="15">
+    <row r="69" spans="1:15" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A69" s="8">
         <v>45982</v>
       </c>
@@ -6186,7 +6195,7 @@
         <v>94</v>
       </c>
       <c r="H69" s="9" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
       <c r="I69" s="9" t="s">
         <v>136</v>
@@ -6210,7 +6219,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="70" spans="1:15" ht="15" hidden="1">
+    <row r="70" spans="1:15" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A70" s="14">
         <v>45982</v>
       </c>
@@ -6257,7 +6266,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="71" spans="1:15" ht="15" hidden="1">
+    <row r="71" spans="1:15" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A71" s="14">
         <v>45982</v>
       </c>
@@ -6304,7 +6313,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="72" spans="1:15" ht="15" hidden="1">
+    <row r="72" spans="1:15" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A72" s="8">
         <v>45982</v>
       </c>
@@ -6351,7 +6360,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="73" spans="1:15" ht="15">
+    <row r="73" spans="1:15" ht="15" x14ac:dyDescent="0.2">
       <c r="A73" s="8">
         <v>45982</v>
       </c>
@@ -6374,7 +6383,7 @@
         <v>170</v>
       </c>
       <c r="H73" s="9" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="I73" s="9" t="s">
         <v>280</v>
@@ -6398,7 +6407,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="74" spans="1:15" ht="15" hidden="1">
+    <row r="74" spans="1:15" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A74" s="8">
         <v>45982</v>
       </c>
@@ -6445,7 +6454,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="75" spans="1:15" ht="15">
+    <row r="75" spans="1:15" ht="15" x14ac:dyDescent="0.2">
       <c r="A75" s="8">
         <v>45982</v>
       </c>
@@ -6492,7 +6501,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="76" spans="1:15" ht="15" hidden="1">
+    <row r="76" spans="1:15" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A76" s="8">
         <v>45982</v>
       </c>
@@ -6539,7 +6548,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="77" spans="1:15" ht="15" hidden="1">
+    <row r="77" spans="1:15" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A77" s="8">
         <v>45982</v>
       </c>
@@ -6586,7 +6595,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="78" spans="1:15" ht="15" hidden="1">
+    <row r="78" spans="1:15" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A78" s="8">
         <v>45982</v>
       </c>
@@ -6633,7 +6642,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="79" spans="1:15" ht="15" hidden="1">
+    <row r="79" spans="1:15" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A79" s="8">
         <v>45982</v>
       </c>
@@ -6680,7 +6689,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="80" spans="1:15" ht="15" hidden="1">
+    <row r="80" spans="1:15" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A80" s="8">
         <v>45982</v>
       </c>
@@ -6727,7 +6736,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="81" spans="1:15" ht="15" hidden="1">
+    <row r="81" spans="1:15" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A81" s="8">
         <v>45982</v>
       </c>
@@ -6774,7 +6783,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="82" spans="1:15" ht="15">
+    <row r="82" spans="1:15" ht="15" x14ac:dyDescent="0.2">
       <c r="A82" s="8">
         <v>45982</v>
       </c>
@@ -6797,7 +6806,7 @@
         <v>284</v>
       </c>
       <c r="H82" s="9" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="I82" s="9" t="s">
         <v>285</v>
@@ -6821,7 +6830,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="83" spans="1:15" ht="15">
+    <row r="83" spans="1:15" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A83" s="8">
         <v>45982</v>
       </c>
@@ -6844,7 +6853,7 @@
         <v>98</v>
       </c>
       <c r="H83" s="9" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="I83" s="9" t="s">
         <v>140</v>
@@ -6868,7 +6877,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="84" spans="1:15" ht="15">
+    <row r="84" spans="1:15" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A84" s="8">
         <v>45982</v>
       </c>
@@ -6891,7 +6900,7 @@
         <v>97</v>
       </c>
       <c r="H84" s="9" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="I84" s="9" t="s">
         <v>139</v>
@@ -6915,7 +6924,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="85" spans="1:15" ht="15" hidden="1">
+    <row r="85" spans="1:15" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A85" s="8">
         <v>45982</v>
       </c>
@@ -6962,7 +6971,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="86" spans="1:15" ht="15" hidden="1">
+    <row r="86" spans="1:15" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A86" s="8">
         <v>45982</v>
       </c>
@@ -7009,7 +7018,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="87" spans="1:15" ht="15" hidden="1">
+    <row r="87" spans="1:15" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A87" s="8">
         <v>45982</v>
       </c>
@@ -7056,7 +7065,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="88" spans="1:15" ht="15" hidden="1">
+    <row r="88" spans="1:15" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A88" s="8">
         <v>45982</v>
       </c>
@@ -7103,7 +7112,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="89" spans="1:15" ht="15" hidden="1">
+    <row r="89" spans="1:15" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A89" s="8">
         <v>45982</v>
       </c>
@@ -7150,7 +7159,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="90" spans="1:15" ht="15" hidden="1">
+    <row r="90" spans="1:15" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A90" s="8">
         <v>45982</v>
       </c>
@@ -7197,7 +7206,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="91" spans="1:15" ht="15" hidden="1">
+    <row r="91" spans="1:15" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A91" s="8">
         <v>45982</v>
       </c>
@@ -7244,7 +7253,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="92" spans="1:15" ht="15" hidden="1">
+    <row r="92" spans="1:15" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A92" s="8">
         <v>45982</v>
       </c>
@@ -7291,7 +7300,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="93" spans="1:15" ht="15" hidden="1">
+    <row r="93" spans="1:15" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A93" s="8">
         <v>45982</v>
       </c>
@@ -7338,7 +7347,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="94" spans="1:15" ht="15" hidden="1">
+    <row r="94" spans="1:15" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A94" s="8">
         <v>45982</v>
       </c>
@@ -7385,7 +7394,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="95" spans="1:15" ht="15" hidden="1">
+    <row r="95" spans="1:15" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A95" s="8">
         <v>45982</v>
       </c>
@@ -7432,7 +7441,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="96" spans="1:15" ht="15" hidden="1">
+    <row r="96" spans="1:15" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A96" s="8">
         <v>45982</v>
       </c>
@@ -7479,7 +7488,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="97" spans="1:15" ht="15" hidden="1">
+    <row r="97" spans="1:15" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A97" s="8">
         <v>45982</v>
       </c>
@@ -7525,6 +7534,21 @@
       <c r="O97" s="4" t="s">
         <v>188</v>
       </c>
+    </row>
+    <row r="101" spans="1:15" ht="15" x14ac:dyDescent="0.2">
+      <c r="D101" s="1"/>
+    </row>
+    <row r="102" spans="1:15" ht="15" x14ac:dyDescent="0.2">
+      <c r="D102" s="1"/>
+    </row>
+    <row r="103" spans="1:15" ht="15" x14ac:dyDescent="0.2">
+      <c r="D103" s="1"/>
+    </row>
+    <row r="104" spans="1:15" ht="15" x14ac:dyDescent="0.2">
+      <c r="D104" s="1"/>
+    </row>
+    <row r="105" spans="1:15" ht="15" x14ac:dyDescent="0.2">
+      <c r="D105" s="1"/>
     </row>
   </sheetData>
   <protectedRanges>
@@ -7533,10 +7557,9 @@
   <autoFilter ref="A1:O97" xr:uid="{F368BCE2-BE99-4B2E-A17A-1E5FAB5A74C3}">
     <filterColumn colId="7">
       <filters blank="1">
-        <filter val="Check"/>
+        <filter val="Fix Stellantis bug"/>
         <filter val="Macro"/>
-        <filter val="Macro + Capping?"/>
-        <filter val="Roberto"/>
+        <filter val="Macro + Capping? + NACE"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -7592,7 +7615,7 @@
       <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
20260210 ESG50 + ESF4P
</commit_message>
<xml_diff>
--- a/GUI + Reviews/New indices list.xlsx
+++ b/GUI + Reviews/New indices list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://euronext-my.sharepoint.com/personal/csonneveld_euronext_com/Documents/Documents/Projects/GUI + Reviews/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="478" documentId="8_{676A6875-F432-47B7-9717-3084B8EAD88C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EB32CA11-16F5-4A9D-B96A-21A34DCCD8E1}"/>
+  <xr:revisionPtr revIDLastSave="528" documentId="8_{676A6875-F432-47B7-9717-3084B8EAD88C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{16AAC1C4-11F9-4F42-9CC9-091FAC378D31}"/>
   <bookViews>
-    <workbookView xWindow="-29370" yWindow="195" windowWidth="29040" windowHeight="15720" xr2:uid="{470E612D-E4A8-42B4-A972-1027153868F9}"/>
+    <workbookView xWindow="-29115" yWindow="-16005" windowWidth="29040" windowHeight="15720" xr2:uid="{470E612D-E4A8-42B4-A972-1027153868F9}"/>
   </bookViews>
   <sheets>
     <sheet name="202512" sheetId="3" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="OLD" sheetId="1" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'202512'!$A$8:$N$58</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'202512'!$A$8:$O$58</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1929" uniqueCount="454">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1960" uniqueCount="483">
   <si>
     <t>EEUS</t>
   </si>
@@ -1403,6 +1403,93 @@
   </si>
   <si>
     <t>Count</t>
+  </si>
+  <si>
+    <t>Review Done</t>
+  </si>
+  <si>
+    <t>Finished</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>EZ3R</t>
+  </si>
+  <si>
+    <t>EBMFP</t>
+  </si>
+  <si>
+    <t>EZ20P</t>
+  </si>
+  <si>
+    <t>EZGP</t>
+  </si>
+  <si>
+    <t>Test With 3 new datapoints and still to be matched</t>
+  </si>
+  <si>
+    <t>IEBMP</t>
+  </si>
+  <si>
+    <t>IECDP</t>
+  </si>
+  <si>
+    <t>IECSP</t>
+  </si>
+  <si>
+    <t>IEENP</t>
+  </si>
+  <si>
+    <t>IEFIP</t>
+  </si>
+  <si>
+    <t>IEHCP</t>
+  </si>
+  <si>
+    <t>IEINP</t>
+  </si>
+  <si>
+    <t>IEREP</t>
+  </si>
+  <si>
+    <t>IEUTP</t>
+  </si>
+  <si>
+    <t>IETLP</t>
+  </si>
+  <si>
+    <t>IETCP</t>
+  </si>
+  <si>
+    <t>IWBMP</t>
+  </si>
+  <si>
+    <t>IWCDP</t>
+  </si>
+  <si>
+    <t>IWCSP</t>
+  </si>
+  <si>
+    <t>IWENP</t>
+  </si>
+  <si>
+    <t>IWFIP</t>
+  </si>
+  <si>
+    <t>IWHCP</t>
+  </si>
+  <si>
+    <t>IWREP</t>
+  </si>
+  <si>
+    <t>IWTCP</t>
+  </si>
+  <si>
+    <t>IWTLP</t>
+  </si>
+  <si>
+    <t>IWUTP</t>
   </si>
 </sst>
 </file>
@@ -1618,7 +1705,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1662,134 +1749,163 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="31">
+  <dxfs count="35">
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FF00FF00"/>
+          <bgColor theme="6" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FF00FF00"/>
+          <bgColor theme="6" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FF00FF00"/>
+          <bgColor theme="6" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FF00FF00"/>
+          <bgColor theme="6" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FF00FF00"/>
+          <bgColor theme="6" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FF00FF00"/>
+          <bgColor theme="6" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FF00FF00"/>
+          <bgColor theme="6" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FF00FF00"/>
+          <bgColor theme="6" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FF00FF00"/>
+          <bgColor theme="6" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FF00FF00"/>
+          <bgColor theme="6" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FF00FF00"/>
+          <bgColor theme="6" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FF00FF00"/>
+          <bgColor theme="6" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FF00FF00"/>
+          <bgColor theme="6" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FF00FF00"/>
+          <bgColor theme="6" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FF00FF00"/>
+          <bgColor theme="6" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FF00FF00"/>
+          <bgColor theme="6" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FF00FF00"/>
+          <bgColor theme="6" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FF00FF00"/>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2218,10 +2334,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F368BCE2-BE99-4B2E-A17A-1E5FAB5A74C3}">
-  <dimension ref="A1:N58"/>
+  <dimension ref="A1:O87"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B81" sqref="B81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -2231,16 +2347,16 @@
     <col min="3" max="3" width="14.125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.75" customWidth="1"/>
-    <col min="6" max="6" width="53.125" customWidth="1"/>
-    <col min="7" max="7" width="21.75" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="53.625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="37.875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.75" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="125.125" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="11.5" customWidth="1"/>
+    <col min="8" max="8" width="21.75" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="53.625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="37.875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.75" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="125.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:15">
       <c r="B1" s="25" t="s">
         <v>116</v>
       </c>
@@ -2248,7 +2364,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:15">
       <c r="B2" s="21" t="s">
         <v>115</v>
       </c>
@@ -2257,7 +2373,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:15">
       <c r="B3" s="21" t="s">
         <v>114</v>
       </c>
@@ -2266,7 +2382,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:15">
       <c r="B4" s="23" t="s">
         <v>106</v>
       </c>
@@ -2275,7 +2391,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="15">
+    <row r="8" spans="1:15" ht="15">
       <c r="A8" s="6" t="s">
         <v>174</v>
       </c>
@@ -2295,31 +2411,34 @@
         <v>116</v>
       </c>
       <c r="G8" s="7" t="s">
+        <v>455</v>
+      </c>
+      <c r="H8" s="7" t="s">
         <v>450</v>
       </c>
-      <c r="H8" s="7" t="s">
+      <c r="I8" s="7" t="s">
         <v>342</v>
       </c>
-      <c r="I8" s="7" t="s">
+      <c r="J8" s="7" t="s">
         <v>179</v>
       </c>
-      <c r="J8" s="7" t="s">
+      <c r="K8" s="7" t="s">
         <v>180</v>
       </c>
-      <c r="K8" s="7" t="s">
+      <c r="L8" s="7" t="s">
         <v>181</v>
       </c>
-      <c r="L8" s="7" t="s">
+      <c r="M8" s="7" t="s">
         <v>182</v>
       </c>
-      <c r="M8" s="7" t="s">
+      <c r="N8" s="7" t="s">
         <v>183</v>
       </c>
-      <c r="N8" s="7" t="s">
+      <c r="O8" s="7" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="15">
+    <row r="9" spans="1:15" ht="15">
       <c r="A9" s="8">
         <v>45982</v>
       </c>
@@ -2338,32 +2457,33 @@
       <c r="F9" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="G9" s="4">
+      <c r="G9" s="4"/>
+      <c r="H9" s="4">
         <v>2</v>
       </c>
-      <c r="H9" s="4" t="s">
+      <c r="I9" s="4" t="s">
         <v>344</v>
       </c>
-      <c r="I9" s="9" t="s">
-        <v>185</v>
-      </c>
-      <c r="J9" s="12" t="s">
+      <c r="J9" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="K9" s="12" t="s">
         <v>233</v>
       </c>
-      <c r="K9" s="12" t="s">
+      <c r="L9" s="12" t="s">
         <v>267</v>
       </c>
-      <c r="L9" s="11" t="s">
-        <v>188</v>
-      </c>
       <c r="M9" s="11" t="s">
-        <v>189</v>
-      </c>
-      <c r="N9" s="4" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" ht="15">
+        <v>188</v>
+      </c>
+      <c r="N9" s="11" t="s">
+        <v>189</v>
+      </c>
+      <c r="O9" s="4" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" ht="15">
       <c r="A10" s="8">
         <v>45982</v>
       </c>
@@ -2382,32 +2502,33 @@
       <c r="F10" s="9" t="s">
         <v>114</v>
       </c>
-      <c r="G10" s="9">
+      <c r="G10" s="9"/>
+      <c r="H10" s="9">
         <v>3</v>
       </c>
-      <c r="H10" s="9" t="s">
+      <c r="I10" s="9" t="s">
         <v>365</v>
       </c>
-      <c r="I10" s="9" t="s">
-        <v>185</v>
-      </c>
-      <c r="J10" s="12" t="s">
+      <c r="J10" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="K10" s="12" t="s">
         <v>366</v>
       </c>
-      <c r="K10" s="12" t="s">
+      <c r="L10" s="12" t="s">
         <v>267</v>
       </c>
-      <c r="L10" s="11" t="s">
-        <v>188</v>
-      </c>
       <c r="M10" s="11" t="s">
-        <v>189</v>
-      </c>
-      <c r="N10" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="N10" s="11" t="s">
+        <v>189</v>
+      </c>
+      <c r="O10" s="4" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="15">
+    <row r="11" spans="1:15" ht="15">
       <c r="A11" s="8">
         <v>45982</v>
       </c>
@@ -2426,32 +2547,33 @@
       <c r="F11" s="9" t="s">
         <v>114</v>
       </c>
-      <c r="G11" s="9">
+      <c r="G11" s="9"/>
+      <c r="H11" s="9">
         <v>1</v>
       </c>
-      <c r="H11" s="9" t="s">
+      <c r="I11" s="9" t="s">
         <v>379</v>
       </c>
-      <c r="I11" s="9" t="s">
-        <v>185</v>
-      </c>
-      <c r="J11" s="12" t="s">
+      <c r="J11" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="K11" s="12" t="s">
         <v>356</v>
       </c>
-      <c r="K11" s="12" t="s">
+      <c r="L11" s="12" t="s">
         <v>267</v>
       </c>
-      <c r="L11" s="11" t="s">
-        <v>188</v>
-      </c>
       <c r="M11" s="11" t="s">
-        <v>189</v>
-      </c>
-      <c r="N11" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="N11" s="11" t="s">
+        <v>189</v>
+      </c>
+      <c r="O11" s="4" t="s">
         <v>380</v>
       </c>
     </row>
-    <row r="12" spans="1:14" ht="15">
+    <row r="12" spans="1:15" ht="15">
       <c r="A12" s="8">
         <v>45982</v>
       </c>
@@ -2470,32 +2592,33 @@
       <c r="F12" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="G12" s="4">
+      <c r="G12" s="4"/>
+      <c r="H12" s="4">
         <v>1</v>
       </c>
-      <c r="H12" s="4" t="s">
+      <c r="I12" s="4" t="s">
         <v>382</v>
       </c>
-      <c r="I12" s="9" t="s">
-        <v>185</v>
-      </c>
-      <c r="J12" s="12" t="s">
+      <c r="J12" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="K12" s="12" t="s">
         <v>356</v>
       </c>
-      <c r="K12" s="12" t="s">
+      <c r="L12" s="12" t="s">
         <v>267</v>
       </c>
-      <c r="L12" s="11" t="s">
-        <v>188</v>
-      </c>
       <c r="M12" s="11" t="s">
-        <v>189</v>
-      </c>
-      <c r="N12" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="N12" s="11" t="s">
+        <v>189</v>
+      </c>
+      <c r="O12" s="4" t="s">
         <v>383</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="15">
+    <row r="13" spans="1:15" ht="15">
       <c r="A13" s="8">
         <v>45982</v>
       </c>
@@ -2514,32 +2637,33 @@
       <c r="F13" s="9" t="s">
         <v>114</v>
       </c>
-      <c r="G13" s="9">
+      <c r="G13" s="9"/>
+      <c r="H13" s="9">
         <v>3</v>
       </c>
-      <c r="H13" s="9" t="s">
+      <c r="I13" s="9" t="s">
         <v>387</v>
       </c>
-      <c r="I13" s="9" t="s">
-        <v>185</v>
-      </c>
-      <c r="J13" s="12" t="s">
+      <c r="J13" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="K13" s="12" t="s">
         <v>366</v>
       </c>
-      <c r="K13" s="12" t="s">
+      <c r="L13" s="12" t="s">
         <v>267</v>
       </c>
-      <c r="L13" s="11" t="s">
-        <v>188</v>
-      </c>
       <c r="M13" s="11" t="s">
-        <v>189</v>
-      </c>
-      <c r="N13" s="4" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" ht="15">
+        <v>188</v>
+      </c>
+      <c r="N13" s="11" t="s">
+        <v>189</v>
+      </c>
+      <c r="O13" s="4" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" ht="15">
       <c r="A14" s="8">
         <v>45982</v>
       </c>
@@ -2558,32 +2682,33 @@
       <c r="F14" s="9" t="s">
         <v>114</v>
       </c>
-      <c r="G14" s="9">
+      <c r="G14" s="9"/>
+      <c r="H14" s="9">
         <v>3</v>
       </c>
-      <c r="H14" s="9" t="s">
+      <c r="I14" s="9" t="s">
         <v>393</v>
       </c>
-      <c r="I14" s="9" t="s">
-        <v>185</v>
-      </c>
-      <c r="J14" s="12" t="s">
+      <c r="J14" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="K14" s="12" t="s">
         <v>106</v>
       </c>
-      <c r="K14" s="12" t="s">
+      <c r="L14" s="12" t="s">
         <v>267</v>
       </c>
-      <c r="L14" s="11" t="s">
-        <v>188</v>
-      </c>
       <c r="M14" s="11" t="s">
-        <v>189</v>
-      </c>
-      <c r="N14" s="4" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" ht="15">
+        <v>188</v>
+      </c>
+      <c r="N14" s="11" t="s">
+        <v>189</v>
+      </c>
+      <c r="O14" s="4" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" ht="15">
       <c r="A15" s="8">
         <v>45982</v>
       </c>
@@ -2602,32 +2727,33 @@
       <c r="F15" s="9" t="s">
         <v>114</v>
       </c>
-      <c r="G15" s="9">
+      <c r="G15" s="9"/>
+      <c r="H15" s="9">
         <v>1</v>
       </c>
-      <c r="H15" s="9" t="s">
+      <c r="I15" s="9" t="s">
         <v>397</v>
       </c>
-      <c r="I15" s="9" t="s">
-        <v>185</v>
-      </c>
-      <c r="J15" s="12" t="s">
+      <c r="J15" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="K15" s="12" t="s">
         <v>168</v>
       </c>
-      <c r="K15" s="12" t="s">
+      <c r="L15" s="12" t="s">
         <v>267</v>
       </c>
-      <c r="L15" s="11" t="s">
-        <v>188</v>
-      </c>
       <c r="M15" s="11" t="s">
-        <v>189</v>
-      </c>
-      <c r="N15" s="4" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" ht="15">
+        <v>188</v>
+      </c>
+      <c r="N15" s="11" t="s">
+        <v>189</v>
+      </c>
+      <c r="O15" s="4" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" ht="15">
       <c r="A16" s="8">
         <v>45982</v>
       </c>
@@ -2646,32 +2772,33 @@
       <c r="F16" s="9" t="s">
         <v>114</v>
       </c>
-      <c r="G16" s="9">
+      <c r="G16" s="9"/>
+      <c r="H16" s="9">
         <v>3</v>
       </c>
-      <c r="H16" s="9" t="s">
+      <c r="I16" s="9" t="s">
         <v>399</v>
       </c>
-      <c r="I16" s="9" t="s">
-        <v>185</v>
-      </c>
-      <c r="J16" s="12" t="s">
+      <c r="J16" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="K16" s="12" t="s">
         <v>106</v>
       </c>
-      <c r="K16" s="12" t="s">
+      <c r="L16" s="12" t="s">
         <v>267</v>
       </c>
-      <c r="L16" s="11" t="s">
-        <v>188</v>
-      </c>
       <c r="M16" s="11" t="s">
-        <v>189</v>
-      </c>
-      <c r="N16" s="4" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14" ht="15">
+        <v>188</v>
+      </c>
+      <c r="N16" s="11" t="s">
+        <v>189</v>
+      </c>
+      <c r="O16" s="4" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" ht="15">
       <c r="A17" s="14">
         <v>45982</v>
       </c>
@@ -2690,32 +2817,33 @@
       <c r="F17" s="15" t="s">
         <v>114</v>
       </c>
-      <c r="G17" s="15">
+      <c r="G17" s="15"/>
+      <c r="H17" s="15">
         <v>3</v>
       </c>
-      <c r="H17" s="15" t="s">
+      <c r="I17" s="15" t="s">
         <v>438</v>
       </c>
-      <c r="I17" s="15" t="s">
+      <c r="J17" s="15" t="s">
         <v>325</v>
       </c>
-      <c r="J17" s="12" t="s">
+      <c r="K17" s="12" t="s">
         <v>114</v>
       </c>
-      <c r="K17" s="12" t="s">
+      <c r="L17" s="12" t="s">
         <v>267</v>
       </c>
-      <c r="L17" s="11" t="s">
-        <v>188</v>
-      </c>
       <c r="M17" s="11" t="s">
-        <v>189</v>
-      </c>
-      <c r="N17" s="4" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14" ht="15">
+        <v>188</v>
+      </c>
+      <c r="N17" s="11" t="s">
+        <v>189</v>
+      </c>
+      <c r="O17" s="4" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" ht="15">
       <c r="A18" s="14">
         <v>45982</v>
       </c>
@@ -2734,32 +2862,33 @@
       <c r="F18" s="15" t="s">
         <v>114</v>
       </c>
-      <c r="G18" s="15">
+      <c r="G18" s="15"/>
+      <c r="H18" s="15">
         <v>3</v>
       </c>
-      <c r="H18" s="15" t="s">
+      <c r="I18" s="15" t="s">
         <v>440</v>
       </c>
-      <c r="I18" s="15" t="s">
-        <v>185</v>
-      </c>
-      <c r="J18" s="12" t="s">
+      <c r="J18" s="15" t="s">
+        <v>185</v>
+      </c>
+      <c r="K18" s="12" t="s">
         <v>356</v>
       </c>
-      <c r="K18" s="12" t="s">
+      <c r="L18" s="12" t="s">
         <v>267</v>
       </c>
-      <c r="L18" s="11" t="s">
-        <v>188</v>
-      </c>
       <c r="M18" s="11" t="s">
-        <v>189</v>
-      </c>
-      <c r="N18" s="4" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14" ht="15">
+        <v>188</v>
+      </c>
+      <c r="N18" s="11" t="s">
+        <v>189</v>
+      </c>
+      <c r="O18" s="4" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" ht="15">
       <c r="A19" s="8">
         <v>46024</v>
       </c>
@@ -2776,30 +2905,31 @@
       <c r="F19" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="G19" s="4">
+      <c r="G19" s="4"/>
+      <c r="H19" s="4">
         <v>1</v>
       </c>
-      <c r="H19" s="4" t="s">
+      <c r="I19" s="4" t="s">
         <v>446</v>
       </c>
-      <c r="I19" s="9" t="s">
+      <c r="J19" s="9" t="s">
         <v>325</v>
       </c>
-      <c r="J19" s="10" t="s">
+      <c r="K19" s="10" t="s">
         <v>447</v>
       </c>
-      <c r="K19" s="10" t="s">
+      <c r="L19" s="10" t="s">
         <v>187</v>
       </c>
-      <c r="L19" s="11" t="s">
-        <v>188</v>
-      </c>
       <c r="M19" s="11" t="s">
-        <v>189</v>
-      </c>
-      <c r="N19" s="4"/>
-    </row>
-    <row r="20" spans="1:14" ht="15">
+        <v>188</v>
+      </c>
+      <c r="N19" s="11" t="s">
+        <v>189</v>
+      </c>
+      <c r="O19" s="4"/>
+    </row>
+    <row r="20" spans="1:15" ht="15">
       <c r="A20" s="8">
         <v>46024</v>
       </c>
@@ -2816,30 +2946,31 @@
       <c r="F20" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="G20" s="4">
+      <c r="G20" s="4"/>
+      <c r="H20" s="4">
         <v>1</v>
       </c>
-      <c r="H20" s="4" t="s">
+      <c r="I20" s="4" t="s">
         <v>446</v>
       </c>
-      <c r="I20" s="9" t="s">
+      <c r="J20" s="9" t="s">
         <v>325</v>
       </c>
-      <c r="J20" s="10" t="s">
+      <c r="K20" s="10" t="s">
         <v>447</v>
       </c>
-      <c r="K20" s="10" t="s">
+      <c r="L20" s="10" t="s">
         <v>187</v>
       </c>
-      <c r="L20" s="11" t="s">
-        <v>188</v>
-      </c>
       <c r="M20" s="11" t="s">
-        <v>189</v>
-      </c>
-      <c r="N20" s="4"/>
-    </row>
-    <row r="21" spans="1:14" ht="15">
+        <v>188</v>
+      </c>
+      <c r="N20" s="11" t="s">
+        <v>189</v>
+      </c>
+      <c r="O20" s="4"/>
+    </row>
+    <row r="21" spans="1:15" ht="15">
       <c r="A21" s="8">
         <v>46024</v>
       </c>
@@ -2856,30 +2987,31 @@
       <c r="F21" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="G21" s="4">
+      <c r="G21" s="4"/>
+      <c r="H21" s="4">
         <v>1</v>
       </c>
-      <c r="H21" s="4" t="s">
+      <c r="I21" s="4" t="s">
         <v>446</v>
       </c>
-      <c r="I21" s="9" t="s">
+      <c r="J21" s="9" t="s">
         <v>325</v>
       </c>
-      <c r="J21" s="10" t="s">
+      <c r="K21" s="10" t="s">
         <v>447</v>
       </c>
-      <c r="K21" s="10" t="s">
+      <c r="L21" s="10" t="s">
         <v>187</v>
       </c>
-      <c r="L21" s="11" t="s">
-        <v>188</v>
-      </c>
       <c r="M21" s="11" t="s">
-        <v>189</v>
-      </c>
-      <c r="N21" s="4"/>
-    </row>
-    <row r="22" spans="1:14" ht="15">
+        <v>188</v>
+      </c>
+      <c r="N21" s="11" t="s">
+        <v>189</v>
+      </c>
+      <c r="O21" s="4"/>
+    </row>
+    <row r="22" spans="1:15" ht="15">
       <c r="A22" s="8">
         <v>46024</v>
       </c>
@@ -2896,30 +3028,31 @@
       <c r="F22" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="G22" s="4">
+      <c r="G22" s="4"/>
+      <c r="H22" s="4">
         <v>1</v>
       </c>
-      <c r="H22" s="4" t="s">
+      <c r="I22" s="4" t="s">
         <v>446</v>
       </c>
-      <c r="I22" s="9" t="s">
+      <c r="J22" s="9" t="s">
         <v>325</v>
       </c>
-      <c r="J22" s="10" t="s">
+      <c r="K22" s="10" t="s">
         <v>447</v>
       </c>
-      <c r="K22" s="10" t="s">
+      <c r="L22" s="10" t="s">
         <v>187</v>
       </c>
-      <c r="L22" s="11" t="s">
-        <v>188</v>
-      </c>
       <c r="M22" s="11" t="s">
-        <v>189</v>
-      </c>
-      <c r="N22" s="4"/>
-    </row>
-    <row r="23" spans="1:14" ht="15">
+        <v>188</v>
+      </c>
+      <c r="N22" s="11" t="s">
+        <v>189</v>
+      </c>
+      <c r="O22" s="4"/>
+    </row>
+    <row r="23" spans="1:15" ht="15">
       <c r="A23" s="8">
         <v>46024</v>
       </c>
@@ -2936,30 +3069,31 @@
       <c r="F23" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="G23" s="4">
+      <c r="G23" s="4"/>
+      <c r="H23" s="4">
         <v>1</v>
       </c>
-      <c r="H23" s="4" t="s">
+      <c r="I23" s="4" t="s">
         <v>446</v>
       </c>
-      <c r="I23" s="9" t="s">
+      <c r="J23" s="9" t="s">
         <v>325</v>
       </c>
-      <c r="J23" s="10" t="s">
+      <c r="K23" s="10" t="s">
         <v>447</v>
       </c>
-      <c r="K23" s="10" t="s">
+      <c r="L23" s="10" t="s">
         <v>187</v>
       </c>
-      <c r="L23" s="11" t="s">
-        <v>188</v>
-      </c>
       <c r="M23" s="11" t="s">
-        <v>189</v>
-      </c>
-      <c r="N23" s="4"/>
-    </row>
-    <row r="24" spans="1:14" ht="15">
+        <v>188</v>
+      </c>
+      <c r="N23" s="11" t="s">
+        <v>189</v>
+      </c>
+      <c r="O23" s="4"/>
+    </row>
+    <row r="24" spans="1:15" ht="15">
       <c r="A24" s="8">
         <v>45982</v>
       </c>
@@ -2979,29 +3113,30 @@
         <v>115</v>
       </c>
       <c r="G24" s="9"/>
-      <c r="H24" s="9" t="s">
+      <c r="H24" s="9"/>
+      <c r="I24" s="9" t="s">
         <v>346</v>
       </c>
-      <c r="I24" s="9" t="s">
+      <c r="J24" s="9" t="s">
         <v>325</v>
       </c>
-      <c r="J24" s="12" t="s">
+      <c r="K24" s="12" t="s">
         <v>106</v>
       </c>
-      <c r="K24" s="12" t="s">
+      <c r="L24" s="12" t="s">
         <v>267</v>
       </c>
-      <c r="L24" s="11" t="s">
-        <v>188</v>
-      </c>
       <c r="M24" s="11" t="s">
-        <v>189</v>
-      </c>
-      <c r="N24" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="N24" s="11" t="s">
+        <v>189</v>
+      </c>
+      <c r="O24" s="4" t="s">
         <v>347</v>
       </c>
     </row>
-    <row r="25" spans="1:14" ht="15">
+    <row r="25" spans="1:15" ht="15">
       <c r="A25" s="8">
         <v>45982</v>
       </c>
@@ -3020,30 +3155,33 @@
       <c r="F25" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="G25" s="9"/>
-      <c r="H25" s="9" t="s">
+      <c r="G25" s="9" t="s">
+        <v>456</v>
+      </c>
+      <c r="H25" s="9"/>
+      <c r="I25" s="9" t="s">
         <v>349</v>
       </c>
-      <c r="I25" s="9" t="s">
+      <c r="J25" s="9" t="s">
         <v>325</v>
       </c>
-      <c r="J25" s="12" t="s">
+      <c r="K25" s="12" t="s">
         <v>114</v>
       </c>
-      <c r="K25" s="12" t="s">
+      <c r="L25" s="12" t="s">
         <v>267</v>
       </c>
-      <c r="L25" s="11" t="s">
-        <v>188</v>
-      </c>
       <c r="M25" s="11" t="s">
-        <v>189</v>
-      </c>
-      <c r="N25" s="4" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="26" spans="1:14" ht="15">
+        <v>188</v>
+      </c>
+      <c r="N25" s="11" t="s">
+        <v>189</v>
+      </c>
+      <c r="O25" s="4" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" ht="15">
       <c r="A26" s="8">
         <v>45982</v>
       </c>
@@ -3062,30 +3200,33 @@
       <c r="F26" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="G26" s="9"/>
-      <c r="H26" s="9" t="s">
+      <c r="G26" s="9" t="s">
+        <v>456</v>
+      </c>
+      <c r="H26" s="9"/>
+      <c r="I26" s="9" t="s">
         <v>351</v>
       </c>
-      <c r="I26" s="9" t="s">
+      <c r="J26" s="9" t="s">
         <v>325</v>
       </c>
-      <c r="J26" s="12" t="s">
+      <c r="K26" s="12" t="s">
         <v>114</v>
       </c>
-      <c r="K26" s="12" t="s">
+      <c r="L26" s="12" t="s">
         <v>267</v>
       </c>
-      <c r="L26" s="11" t="s">
-        <v>188</v>
-      </c>
       <c r="M26" s="11" t="s">
-        <v>189</v>
-      </c>
-      <c r="N26" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="N26" s="11" t="s">
+        <v>189</v>
+      </c>
+      <c r="O26" s="4" t="s">
         <v>352</v>
       </c>
     </row>
-    <row r="27" spans="1:14" ht="15">
+    <row r="27" spans="1:15" ht="15">
       <c r="A27" s="8">
         <v>45982</v>
       </c>
@@ -3105,29 +3246,30 @@
         <v>115</v>
       </c>
       <c r="G27" s="9"/>
-      <c r="H27" s="9" t="s">
+      <c r="H27" s="9"/>
+      <c r="I27" s="9" t="s">
         <v>354</v>
       </c>
-      <c r="I27" s="9" t="s">
+      <c r="J27" s="9" t="s">
         <v>325</v>
       </c>
-      <c r="J27" s="12" t="s">
+      <c r="K27" s="12" t="s">
         <v>106</v>
       </c>
-      <c r="K27" s="12" t="s">
+      <c r="L27" s="12" t="s">
         <v>267</v>
       </c>
-      <c r="L27" s="11" t="s">
-        <v>188</v>
-      </c>
       <c r="M27" s="11" t="s">
-        <v>189</v>
-      </c>
-      <c r="N27" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="N27" s="11" t="s">
+        <v>189</v>
+      </c>
+      <c r="O27" s="4" t="s">
         <v>355</v>
       </c>
     </row>
-    <row r="28" spans="1:14" ht="15">
+    <row r="28" spans="1:15" ht="15">
       <c r="A28" s="8">
         <v>45982</v>
       </c>
@@ -3147,29 +3289,30 @@
         <v>115</v>
       </c>
       <c r="G28" s="9"/>
-      <c r="H28" s="9" t="s">
+      <c r="H28" s="9"/>
+      <c r="I28" s="9" t="s">
         <v>360</v>
       </c>
-      <c r="I28" s="9" t="s">
+      <c r="J28" s="9" t="s">
         <v>325</v>
       </c>
-      <c r="J28" s="12" t="s">
+      <c r="K28" s="12" t="s">
         <v>114</v>
       </c>
-      <c r="K28" s="12" t="s">
+      <c r="L28" s="12" t="s">
         <v>267</v>
       </c>
-      <c r="L28" s="11" t="s">
-        <v>188</v>
-      </c>
       <c r="M28" s="11" t="s">
-        <v>189</v>
-      </c>
-      <c r="N28" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="N28" s="11" t="s">
+        <v>189</v>
+      </c>
+      <c r="O28" s="4" t="s">
         <v>361</v>
       </c>
     </row>
-    <row r="29" spans="1:14" ht="15">
+    <row r="29" spans="1:15" ht="15">
       <c r="A29" s="8">
         <v>45982</v>
       </c>
@@ -3189,29 +3332,30 @@
         <v>115</v>
       </c>
       <c r="G29" s="9"/>
-      <c r="H29" s="9" t="s">
+      <c r="H29" s="9"/>
+      <c r="I29" s="9" t="s">
         <v>363</v>
       </c>
-      <c r="I29" s="9" t="s">
+      <c r="J29" s="9" t="s">
         <v>325</v>
       </c>
-      <c r="J29" s="12" t="s">
+      <c r="K29" s="12" t="s">
         <v>114</v>
       </c>
-      <c r="K29" s="12" t="s">
+      <c r="L29" s="12" t="s">
         <v>267</v>
       </c>
-      <c r="L29" s="11" t="s">
-        <v>188</v>
-      </c>
       <c r="M29" s="11" t="s">
-        <v>189</v>
-      </c>
-      <c r="N29" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="N29" s="11" t="s">
+        <v>189</v>
+      </c>
+      <c r="O29" s="4" t="s">
         <v>361</v>
       </c>
     </row>
-    <row r="30" spans="1:14" ht="15">
+    <row r="30" spans="1:15" ht="15">
       <c r="A30" s="8">
         <v>45982</v>
       </c>
@@ -3231,29 +3375,30 @@
         <v>115</v>
       </c>
       <c r="G30" s="9"/>
-      <c r="H30" s="9" t="s">
+      <c r="H30" s="9"/>
+      <c r="I30" s="9" t="s">
         <v>376</v>
       </c>
-      <c r="I30" s="9" t="s">
+      <c r="J30" s="9" t="s">
         <v>325</v>
       </c>
-      <c r="J30" s="12" t="s">
+      <c r="K30" s="12" t="s">
         <v>114</v>
       </c>
-      <c r="K30" s="12" t="s">
+      <c r="L30" s="12" t="s">
         <v>267</v>
       </c>
-      <c r="L30" s="11" t="s">
-        <v>188</v>
-      </c>
       <c r="M30" s="11" t="s">
-        <v>189</v>
-      </c>
-      <c r="N30" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="N30" s="11" t="s">
+        <v>189</v>
+      </c>
+      <c r="O30" s="4" t="s">
         <v>377</v>
       </c>
     </row>
-    <row r="31" spans="1:14" ht="15">
+    <row r="31" spans="1:15" ht="15">
       <c r="A31" s="8">
         <v>45982</v>
       </c>
@@ -3273,29 +3418,30 @@
         <v>115</v>
       </c>
       <c r="G31" s="9"/>
-      <c r="H31" s="9" t="s">
+      <c r="H31" s="9"/>
+      <c r="I31" s="9" t="s">
         <v>389</v>
       </c>
-      <c r="I31" s="9" t="s">
-        <v>185</v>
-      </c>
-      <c r="J31" s="12" t="s">
+      <c r="J31" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="K31" s="12" t="s">
         <v>358</v>
       </c>
-      <c r="K31" s="12" t="s">
+      <c r="L31" s="12" t="s">
         <v>267</v>
       </c>
-      <c r="L31" s="11" t="s">
-        <v>188</v>
-      </c>
       <c r="M31" s="11" t="s">
-        <v>189</v>
-      </c>
-      <c r="N31" s="4" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="32" spans="1:14" ht="15">
+        <v>188</v>
+      </c>
+      <c r="N31" s="11" t="s">
+        <v>189</v>
+      </c>
+      <c r="O31" s="4" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" ht="15">
       <c r="A32" s="8">
         <v>45982</v>
       </c>
@@ -3315,29 +3461,30 @@
         <v>115</v>
       </c>
       <c r="G32" s="9"/>
-      <c r="H32" s="9" t="s">
+      <c r="H32" s="9"/>
+      <c r="I32" s="9" t="s">
         <v>391</v>
       </c>
-      <c r="I32" s="9" t="s">
-        <v>185</v>
-      </c>
-      <c r="J32" s="12" t="s">
+      <c r="J32" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="K32" s="12" t="s">
         <v>168</v>
       </c>
-      <c r="K32" s="12" t="s">
+      <c r="L32" s="12" t="s">
         <v>267</v>
       </c>
-      <c r="L32" s="11" t="s">
-        <v>188</v>
-      </c>
       <c r="M32" s="11" t="s">
-        <v>189</v>
-      </c>
-      <c r="N32" s="4" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="33" spans="1:14" ht="15">
+        <v>188</v>
+      </c>
+      <c r="N32" s="11" t="s">
+        <v>189</v>
+      </c>
+      <c r="O32" s="4" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" ht="15">
       <c r="A33" s="8">
         <v>45982</v>
       </c>
@@ -3356,32 +3503,33 @@
       <c r="F33" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="G33" s="9" t="s">
+      <c r="G33" s="9"/>
+      <c r="H33" s="9" t="s">
         <v>448</v>
       </c>
-      <c r="H33" s="9" t="s">
+      <c r="I33" s="9" t="s">
         <v>403</v>
       </c>
-      <c r="I33" s="9" t="s">
-        <v>185</v>
-      </c>
-      <c r="J33" s="12" t="s">
+      <c r="J33" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="K33" s="12" t="s">
         <v>168</v>
       </c>
-      <c r="K33" s="12" t="s">
+      <c r="L33" s="12" t="s">
         <v>267</v>
       </c>
-      <c r="L33" s="11" t="s">
-        <v>188</v>
-      </c>
       <c r="M33" s="11" t="s">
-        <v>189</v>
-      </c>
-      <c r="N33" s="4" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="34" spans="1:14" ht="15">
+        <v>188</v>
+      </c>
+      <c r="N33" s="11" t="s">
+        <v>189</v>
+      </c>
+      <c r="O33" s="4" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" ht="15">
       <c r="A34" s="8">
         <v>45982</v>
       </c>
@@ -3401,29 +3549,30 @@
         <v>115</v>
       </c>
       <c r="G34" s="9"/>
-      <c r="H34" s="9" t="s">
+      <c r="H34" s="9"/>
+      <c r="I34" s="9" t="s">
         <v>405</v>
       </c>
-      <c r="I34" s="9" t="s">
-        <v>185</v>
-      </c>
-      <c r="J34" s="12" t="s">
+      <c r="J34" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="K34" s="12" t="s">
         <v>114</v>
       </c>
-      <c r="K34" s="12" t="s">
+      <c r="L34" s="12" t="s">
         <v>267</v>
       </c>
-      <c r="L34" s="11" t="s">
-        <v>188</v>
-      </c>
       <c r="M34" s="11" t="s">
-        <v>189</v>
-      </c>
-      <c r="N34" s="4" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="35" spans="1:14" ht="15">
+        <v>188</v>
+      </c>
+      <c r="N34" s="11" t="s">
+        <v>189</v>
+      </c>
+      <c r="O34" s="4" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" ht="15">
       <c r="A35" s="8">
         <v>45982</v>
       </c>
@@ -3443,29 +3592,30 @@
         <v>115</v>
       </c>
       <c r="G35" s="9"/>
-      <c r="H35" s="9" t="s">
+      <c r="H35" s="9"/>
+      <c r="I35" s="9" t="s">
         <v>407</v>
       </c>
-      <c r="I35" s="9" t="s">
+      <c r="J35" s="9" t="s">
         <v>325</v>
       </c>
-      <c r="J35" s="12" t="s">
+      <c r="K35" s="12" t="s">
         <v>357</v>
       </c>
-      <c r="K35" s="12" t="s">
+      <c r="L35" s="12" t="s">
         <v>267</v>
       </c>
-      <c r="L35" s="11" t="s">
-        <v>188</v>
-      </c>
       <c r="M35" s="11" t="s">
-        <v>189</v>
-      </c>
-      <c r="N35" s="4" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="36" spans="1:14" ht="15">
+        <v>188</v>
+      </c>
+      <c r="N35" s="11" t="s">
+        <v>189</v>
+      </c>
+      <c r="O35" s="4" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" ht="15">
       <c r="A36" s="8">
         <v>45982</v>
       </c>
@@ -3485,29 +3635,30 @@
         <v>115</v>
       </c>
       <c r="G36" s="9"/>
-      <c r="H36" s="4" t="s">
+      <c r="H36" s="9"/>
+      <c r="I36" s="4" t="s">
         <v>409</v>
       </c>
-      <c r="I36" s="9" t="s">
+      <c r="J36" s="9" t="s">
         <v>325</v>
       </c>
-      <c r="J36" s="12" t="s">
+      <c r="K36" s="12" t="s">
         <v>357</v>
       </c>
-      <c r="K36" s="12" t="s">
+      <c r="L36" s="12" t="s">
         <v>267</v>
       </c>
-      <c r="L36" s="11" t="s">
-        <v>188</v>
-      </c>
       <c r="M36" s="11" t="s">
-        <v>189</v>
-      </c>
-      <c r="N36" s="4" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="37" spans="1:14" ht="15">
+        <v>188</v>
+      </c>
+      <c r="N36" s="11" t="s">
+        <v>189</v>
+      </c>
+      <c r="O36" s="4" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" ht="15">
       <c r="A37" s="8">
         <v>45982</v>
       </c>
@@ -3527,29 +3678,30 @@
         <v>115</v>
       </c>
       <c r="G37" s="9"/>
-      <c r="H37" s="9" t="s">
+      <c r="H37" s="9"/>
+      <c r="I37" s="9" t="s">
         <v>411</v>
       </c>
-      <c r="I37" s="9" t="s">
+      <c r="J37" s="9" t="s">
         <v>325</v>
       </c>
-      <c r="J37" s="12" t="s">
+      <c r="K37" s="12" t="s">
         <v>357</v>
       </c>
-      <c r="K37" s="12" t="s">
+      <c r="L37" s="12" t="s">
         <v>267</v>
       </c>
-      <c r="L37" s="13" t="s">
-        <v>188</v>
-      </c>
       <c r="M37" s="13" t="s">
-        <v>189</v>
-      </c>
-      <c r="N37" s="4" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="38" spans="1:14" ht="15">
+        <v>188</v>
+      </c>
+      <c r="N37" s="13" t="s">
+        <v>189</v>
+      </c>
+      <c r="O37" s="4" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" ht="15">
       <c r="A38" s="8">
         <v>45982</v>
       </c>
@@ -3569,29 +3721,30 @@
         <v>115</v>
       </c>
       <c r="G38" s="9"/>
-      <c r="H38" s="9" t="s">
+      <c r="H38" s="9"/>
+      <c r="I38" s="9" t="s">
         <v>413</v>
       </c>
-      <c r="I38" s="9" t="s">
+      <c r="J38" s="9" t="s">
         <v>325</v>
       </c>
-      <c r="J38" s="12" t="s">
+      <c r="K38" s="12" t="s">
         <v>357</v>
       </c>
-      <c r="K38" s="12" t="s">
+      <c r="L38" s="12" t="s">
         <v>267</v>
       </c>
-      <c r="L38" s="11" t="s">
-        <v>188</v>
-      </c>
       <c r="M38" s="11" t="s">
-        <v>189</v>
-      </c>
-      <c r="N38" s="4" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="39" spans="1:14" ht="15">
+        <v>188</v>
+      </c>
+      <c r="N38" s="11" t="s">
+        <v>189</v>
+      </c>
+      <c r="O38" s="4" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" ht="15">
       <c r="A39" s="8">
         <v>45982</v>
       </c>
@@ -3611,29 +3764,30 @@
         <v>115</v>
       </c>
       <c r="G39" s="9"/>
-      <c r="H39" s="9" t="s">
+      <c r="H39" s="9"/>
+      <c r="I39" s="9" t="s">
         <v>415</v>
       </c>
-      <c r="I39" s="9" t="s">
+      <c r="J39" s="9" t="s">
         <v>325</v>
       </c>
-      <c r="J39" s="12" t="s">
+      <c r="K39" s="12" t="s">
         <v>357</v>
       </c>
-      <c r="K39" s="12" t="s">
+      <c r="L39" s="12" t="s">
         <v>267</v>
       </c>
-      <c r="L39" s="11" t="s">
-        <v>188</v>
-      </c>
       <c r="M39" s="11" t="s">
-        <v>189</v>
-      </c>
-      <c r="N39" s="4" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="40" spans="1:14" ht="15">
+        <v>188</v>
+      </c>
+      <c r="N39" s="11" t="s">
+        <v>189</v>
+      </c>
+      <c r="O39" s="4" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" ht="15">
       <c r="A40" s="8">
         <v>45982</v>
       </c>
@@ -3653,29 +3807,30 @@
         <v>115</v>
       </c>
       <c r="G40" s="9"/>
-      <c r="H40" s="9" t="s">
+      <c r="H40" s="9"/>
+      <c r="I40" s="9" t="s">
         <v>417</v>
       </c>
-      <c r="I40" s="9" t="s">
+      <c r="J40" s="9" t="s">
         <v>325</v>
       </c>
-      <c r="J40" s="12" t="s">
+      <c r="K40" s="12" t="s">
         <v>357</v>
       </c>
-      <c r="K40" s="12" t="s">
+      <c r="L40" s="12" t="s">
         <v>267</v>
       </c>
-      <c r="L40" s="11" t="s">
-        <v>188</v>
-      </c>
       <c r="M40" s="11" t="s">
-        <v>189</v>
-      </c>
-      <c r="N40" s="4" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="41" spans="1:14" ht="15">
+        <v>188</v>
+      </c>
+      <c r="N40" s="11" t="s">
+        <v>189</v>
+      </c>
+      <c r="O40" s="4" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" ht="15">
       <c r="A41" s="8">
         <v>45982</v>
       </c>
@@ -3695,29 +3850,30 @@
         <v>115</v>
       </c>
       <c r="G41" s="9"/>
-      <c r="H41" s="9" t="s">
+      <c r="H41" s="9"/>
+      <c r="I41" s="9" t="s">
         <v>419</v>
       </c>
-      <c r="I41" s="9" t="s">
+      <c r="J41" s="9" t="s">
         <v>325</v>
       </c>
-      <c r="J41" s="12" t="s">
+      <c r="K41" s="12" t="s">
         <v>357</v>
       </c>
-      <c r="K41" s="12" t="s">
+      <c r="L41" s="12" t="s">
         <v>267</v>
       </c>
-      <c r="L41" s="11" t="s">
-        <v>188</v>
-      </c>
       <c r="M41" s="11" t="s">
-        <v>189</v>
-      </c>
-      <c r="N41" s="4" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="42" spans="1:14" ht="15">
+        <v>188</v>
+      </c>
+      <c r="N41" s="11" t="s">
+        <v>189</v>
+      </c>
+      <c r="O41" s="4" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" ht="15">
       <c r="A42" s="8">
         <v>45982</v>
       </c>
@@ -3737,29 +3893,30 @@
         <v>115</v>
       </c>
       <c r="G42" s="9"/>
-      <c r="H42" s="9" t="s">
+      <c r="H42" s="9"/>
+      <c r="I42" s="9" t="s">
         <v>421</v>
       </c>
-      <c r="I42" s="9" t="s">
+      <c r="J42" s="9" t="s">
         <v>325</v>
       </c>
-      <c r="J42" s="12" t="s">
+      <c r="K42" s="12" t="s">
         <v>357</v>
       </c>
-      <c r="K42" s="12" t="s">
+      <c r="L42" s="12" t="s">
         <v>267</v>
       </c>
-      <c r="L42" s="11" t="s">
-        <v>188</v>
-      </c>
       <c r="M42" s="11" t="s">
-        <v>189</v>
-      </c>
-      <c r="N42" s="4" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="43" spans="1:14" ht="15">
+        <v>188</v>
+      </c>
+      <c r="N42" s="11" t="s">
+        <v>189</v>
+      </c>
+      <c r="O42" s="4" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" ht="15">
       <c r="A43" s="8">
         <v>45982</v>
       </c>
@@ -3779,29 +3936,30 @@
         <v>115</v>
       </c>
       <c r="G43" s="9"/>
-      <c r="H43" s="9" t="s">
+      <c r="H43" s="9"/>
+      <c r="I43" s="9" t="s">
         <v>423</v>
       </c>
-      <c r="I43" s="9" t="s">
+      <c r="J43" s="9" t="s">
         <v>325</v>
       </c>
-      <c r="J43" s="12" t="s">
+      <c r="K43" s="12" t="s">
         <v>357</v>
       </c>
-      <c r="K43" s="12" t="s">
+      <c r="L43" s="12" t="s">
         <v>267</v>
       </c>
-      <c r="L43" s="11" t="s">
-        <v>188</v>
-      </c>
       <c r="M43" s="11" t="s">
-        <v>189</v>
-      </c>
-      <c r="N43" s="4" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="44" spans="1:14" ht="15">
+        <v>188</v>
+      </c>
+      <c r="N43" s="11" t="s">
+        <v>189</v>
+      </c>
+      <c r="O43" s="4" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" ht="15">
       <c r="A44" s="8">
         <v>45982</v>
       </c>
@@ -3821,29 +3979,30 @@
         <v>115</v>
       </c>
       <c r="G44" s="9"/>
-      <c r="H44" s="9" t="s">
+      <c r="H44" s="9"/>
+      <c r="I44" s="9" t="s">
         <v>425</v>
       </c>
-      <c r="I44" s="9" t="s">
+      <c r="J44" s="9" t="s">
         <v>325</v>
       </c>
-      <c r="J44" s="12" t="s">
+      <c r="K44" s="12" t="s">
         <v>357</v>
       </c>
-      <c r="K44" s="12" t="s">
+      <c r="L44" s="12" t="s">
         <v>267</v>
       </c>
-      <c r="L44" s="13" t="s">
-        <v>188</v>
-      </c>
       <c r="M44" s="13" t="s">
-        <v>189</v>
-      </c>
-      <c r="N44" s="4" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="45" spans="1:14" ht="15">
+        <v>188</v>
+      </c>
+      <c r="N44" s="13" t="s">
+        <v>189</v>
+      </c>
+      <c r="O44" s="4" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" ht="15">
       <c r="A45" s="8">
         <v>45982</v>
       </c>
@@ -3862,32 +4021,33 @@
       <c r="F45" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="G45" s="9" t="s">
+      <c r="G45" s="9"/>
+      <c r="H45" s="9" t="s">
         <v>448</v>
       </c>
-      <c r="H45" s="9" t="s">
+      <c r="I45" s="9" t="s">
         <v>427</v>
       </c>
-      <c r="I45" s="9" t="s">
-        <v>185</v>
-      </c>
-      <c r="J45" s="12" t="s">
+      <c r="J45" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="K45" s="12" t="s">
         <v>428</v>
       </c>
-      <c r="K45" s="12" t="s">
+      <c r="L45" s="12" t="s">
         <v>267</v>
       </c>
-      <c r="L45" s="11" t="s">
-        <v>188</v>
-      </c>
       <c r="M45" s="11" t="s">
-        <v>189</v>
-      </c>
-      <c r="N45" s="4" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="46" spans="1:14" ht="15">
+        <v>188</v>
+      </c>
+      <c r="N45" s="11" t="s">
+        <v>189</v>
+      </c>
+      <c r="O45" s="4" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15" ht="15">
       <c r="A46" s="8">
         <v>45982</v>
       </c>
@@ -3906,32 +4066,33 @@
       <c r="F46" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="G46" s="9" t="s">
+      <c r="G46" s="9"/>
+      <c r="H46" s="9" t="s">
         <v>448</v>
       </c>
-      <c r="H46" s="9" t="s">
+      <c r="I46" s="9" t="s">
         <v>430</v>
       </c>
-      <c r="I46" s="9" t="s">
-        <v>185</v>
-      </c>
-      <c r="J46" s="12" t="s">
+      <c r="J46" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="K46" s="12" t="s">
         <v>356</v>
       </c>
-      <c r="K46" s="12" t="s">
+      <c r="L46" s="12" t="s">
         <v>267</v>
       </c>
-      <c r="L46" s="11" t="s">
-        <v>188</v>
-      </c>
       <c r="M46" s="11" t="s">
-        <v>189</v>
-      </c>
-      <c r="N46" s="4" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="47" spans="1:14" ht="15">
+        <v>188</v>
+      </c>
+      <c r="N46" s="11" t="s">
+        <v>189</v>
+      </c>
+      <c r="O46" s="4" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15" ht="15">
       <c r="A47" s="8">
         <v>45982</v>
       </c>
@@ -3950,32 +4111,33 @@
       <c r="F47" s="9" t="s">
         <v>106</v>
       </c>
-      <c r="G47" s="9">
+      <c r="G47" s="9"/>
+      <c r="H47" s="9">
         <v>1</v>
       </c>
-      <c r="H47" s="9" t="s">
+      <c r="I47" s="9" t="s">
         <v>368</v>
       </c>
-      <c r="I47" s="9" t="s">
-        <v>185</v>
-      </c>
-      <c r="J47" s="12" t="s">
+      <c r="J47" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="K47" s="12" t="s">
         <v>356</v>
       </c>
-      <c r="K47" s="12" t="s">
+      <c r="L47" s="12" t="s">
         <v>267</v>
       </c>
-      <c r="L47" s="11" t="s">
-        <v>188</v>
-      </c>
       <c r="M47" s="11" t="s">
-        <v>189</v>
-      </c>
-      <c r="N47" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="N47" s="11" t="s">
+        <v>189</v>
+      </c>
+      <c r="O47" s="4" t="s">
         <v>369</v>
       </c>
     </row>
-    <row r="48" spans="1:14" ht="15">
+    <row r="48" spans="1:15" ht="15">
       <c r="A48" s="8">
         <v>45982</v>
       </c>
@@ -3994,32 +4156,33 @@
       <c r="F48" s="9" t="s">
         <v>106</v>
       </c>
-      <c r="G48" s="9">
+      <c r="G48" s="9"/>
+      <c r="H48" s="9">
         <v>1</v>
       </c>
-      <c r="H48" s="9" t="s">
+      <c r="I48" s="9" t="s">
         <v>371</v>
       </c>
-      <c r="I48" s="9" t="s">
-        <v>185</v>
-      </c>
-      <c r="J48" s="12" t="s">
+      <c r="J48" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="K48" s="12" t="s">
         <v>356</v>
       </c>
-      <c r="K48" s="12" t="s">
+      <c r="L48" s="12" t="s">
         <v>267</v>
       </c>
-      <c r="L48" s="11" t="s">
-        <v>188</v>
-      </c>
       <c r="M48" s="11" t="s">
-        <v>189</v>
-      </c>
-      <c r="N48" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="N48" s="11" t="s">
+        <v>189</v>
+      </c>
+      <c r="O48" s="4" t="s">
         <v>372</v>
       </c>
     </row>
-    <row r="49" spans="1:14" ht="15">
+    <row r="49" spans="1:15" ht="15">
       <c r="A49" s="8">
         <v>45982</v>
       </c>
@@ -4038,32 +4201,33 @@
       <c r="F49" s="9" t="s">
         <v>106</v>
       </c>
-      <c r="G49" s="9">
+      <c r="G49" s="9"/>
+      <c r="H49" s="9">
         <v>1</v>
       </c>
-      <c r="H49" s="9" t="s">
+      <c r="I49" s="9" t="s">
         <v>374</v>
       </c>
-      <c r="I49" s="9" t="s">
-        <v>185</v>
-      </c>
-      <c r="J49" s="12" t="s">
+      <c r="J49" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="K49" s="12" t="s">
         <v>356</v>
       </c>
-      <c r="K49" s="12" t="s">
+      <c r="L49" s="12" t="s">
         <v>267</v>
       </c>
-      <c r="L49" s="13" t="s">
-        <v>188</v>
-      </c>
       <c r="M49" s="13" t="s">
-        <v>189</v>
-      </c>
-      <c r="N49" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="N49" s="13" t="s">
+        <v>189</v>
+      </c>
+      <c r="O49" s="4" t="s">
         <v>372</v>
       </c>
     </row>
-    <row r="50" spans="1:14" ht="15">
+    <row r="50" spans="1:15" ht="15">
       <c r="A50" s="8">
         <v>45982</v>
       </c>
@@ -4082,32 +4246,33 @@
       <c r="F50" s="9" t="s">
         <v>106</v>
       </c>
-      <c r="G50" s="9">
+      <c r="G50" s="9"/>
+      <c r="H50" s="9">
         <v>2</v>
       </c>
-      <c r="H50" s="9" t="s">
+      <c r="I50" s="9" t="s">
         <v>385</v>
       </c>
-      <c r="I50" s="9" t="s">
-        <v>185</v>
-      </c>
-      <c r="J50" s="12" t="s">
+      <c r="J50" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="K50" s="12" t="s">
         <v>366</v>
       </c>
-      <c r="K50" s="12" t="s">
+      <c r="L50" s="12" t="s">
         <v>267</v>
       </c>
-      <c r="L50" s="13" t="s">
-        <v>188</v>
-      </c>
       <c r="M50" s="13" t="s">
-        <v>189</v>
-      </c>
-      <c r="N50" s="4" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="51" spans="1:14" ht="15">
+        <v>188</v>
+      </c>
+      <c r="N50" s="13" t="s">
+        <v>189</v>
+      </c>
+      <c r="O50" s="4" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="51" spans="1:15" ht="15">
       <c r="A51" s="8">
         <v>45982</v>
       </c>
@@ -4126,32 +4291,33 @@
       <c r="F51" s="9" t="s">
         <v>106</v>
       </c>
-      <c r="G51" s="9">
+      <c r="G51" s="9"/>
+      <c r="H51" s="9">
         <v>2</v>
       </c>
-      <c r="H51" s="9" t="s">
+      <c r="I51" s="9" t="s">
         <v>395</v>
       </c>
-      <c r="I51" s="9" t="s">
-        <v>185</v>
-      </c>
-      <c r="J51" s="12" t="s">
+      <c r="J51" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="K51" s="12" t="s">
         <v>106</v>
       </c>
-      <c r="K51" s="12" t="s">
+      <c r="L51" s="12" t="s">
         <v>267</v>
       </c>
-      <c r="L51" s="11" t="s">
-        <v>188</v>
-      </c>
       <c r="M51" s="11" t="s">
-        <v>189</v>
-      </c>
-      <c r="N51" s="4" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="52" spans="1:14" ht="15">
+        <v>188</v>
+      </c>
+      <c r="N51" s="11" t="s">
+        <v>189</v>
+      </c>
+      <c r="O51" s="4" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="52" spans="1:15" ht="15">
       <c r="A52" s="8">
         <v>45982</v>
       </c>
@@ -4170,32 +4336,33 @@
       <c r="F52" s="9" t="s">
         <v>106</v>
       </c>
-      <c r="G52" s="9">
+      <c r="G52" s="9"/>
+      <c r="H52" s="9">
         <v>3</v>
       </c>
-      <c r="H52" s="9" t="s">
+      <c r="I52" s="9" t="s">
         <v>401</v>
       </c>
-      <c r="I52" s="9" t="s">
-        <v>185</v>
-      </c>
-      <c r="J52" s="12" t="s">
+      <c r="J52" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="K52" s="12" t="s">
         <v>106</v>
       </c>
-      <c r="K52" s="12" t="s">
+      <c r="L52" s="12" t="s">
         <v>267</v>
       </c>
-      <c r="L52" s="11" t="s">
-        <v>188</v>
-      </c>
       <c r="M52" s="11" t="s">
-        <v>189</v>
-      </c>
-      <c r="N52" s="4" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="53" spans="1:14" ht="15">
+        <v>188</v>
+      </c>
+      <c r="N52" s="11" t="s">
+        <v>189</v>
+      </c>
+      <c r="O52" s="4" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="53" spans="1:15" ht="15">
       <c r="A53" s="8">
         <v>45982</v>
       </c>
@@ -4214,32 +4381,33 @@
       <c r="F53" s="9" t="s">
         <v>106</v>
       </c>
-      <c r="G53" s="9">
+      <c r="G53" s="9"/>
+      <c r="H53" s="9">
         <v>2</v>
       </c>
-      <c r="H53" s="9" t="s">
+      <c r="I53" s="9" t="s">
         <v>432</v>
       </c>
-      <c r="I53" s="9" t="s">
-        <v>185</v>
-      </c>
-      <c r="J53" s="12" t="s">
+      <c r="J53" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="K53" s="12" t="s">
         <v>356</v>
       </c>
-      <c r="K53" s="12" t="s">
+      <c r="L53" s="12" t="s">
         <v>267</v>
       </c>
-      <c r="L53" s="11" t="s">
-        <v>188</v>
-      </c>
       <c r="M53" s="11" t="s">
-        <v>189</v>
-      </c>
-      <c r="N53" s="4" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="54" spans="1:14" ht="15">
+        <v>188</v>
+      </c>
+      <c r="N53" s="11" t="s">
+        <v>189</v>
+      </c>
+      <c r="O53" s="4" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="54" spans="1:15" ht="15">
       <c r="A54" s="8">
         <v>45982</v>
       </c>
@@ -4258,32 +4426,33 @@
       <c r="F54" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="G54" s="4">
+      <c r="G54" s="4"/>
+      <c r="H54" s="4">
         <v>2</v>
       </c>
-      <c r="H54" s="4" t="s">
+      <c r="I54" s="4" t="s">
         <v>434</v>
       </c>
-      <c r="I54" s="9" t="s">
-        <v>185</v>
-      </c>
-      <c r="J54" s="12" t="s">
+      <c r="J54" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="K54" s="12" t="s">
         <v>356</v>
       </c>
-      <c r="K54" s="12" t="s">
+      <c r="L54" s="12" t="s">
         <v>267</v>
       </c>
-      <c r="L54" s="11" t="s">
-        <v>188</v>
-      </c>
       <c r="M54" s="11" t="s">
-        <v>189</v>
-      </c>
-      <c r="N54" s="4" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="55" spans="1:14" ht="15">
+        <v>188</v>
+      </c>
+      <c r="N54" s="11" t="s">
+        <v>189</v>
+      </c>
+      <c r="O54" s="4" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="55" spans="1:15" ht="15">
       <c r="A55" s="8">
         <v>45982</v>
       </c>
@@ -4302,32 +4471,33 @@
       <c r="F55" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="G55" s="4">
+      <c r="G55" s="4"/>
+      <c r="H55" s="4">
         <v>2</v>
       </c>
-      <c r="H55" s="4" t="s">
+      <c r="I55" s="4" t="s">
         <v>436</v>
       </c>
-      <c r="I55" s="9" t="s">
-        <v>185</v>
-      </c>
-      <c r="J55" s="12" t="s">
+      <c r="J55" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="K55" s="12" t="s">
         <v>356</v>
       </c>
-      <c r="K55" s="12" t="s">
+      <c r="L55" s="12" t="s">
         <v>267</v>
       </c>
-      <c r="L55" s="11" t="s">
-        <v>188</v>
-      </c>
       <c r="M55" s="11" t="s">
-        <v>189</v>
-      </c>
-      <c r="N55" s="4" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="56" spans="1:14" ht="15">
+        <v>188</v>
+      </c>
+      <c r="N55" s="11" t="s">
+        <v>189</v>
+      </c>
+      <c r="O55" s="4" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="56" spans="1:15" ht="15">
       <c r="A56" s="8">
         <v>45982</v>
       </c>
@@ -4346,32 +4516,33 @@
       <c r="F56" s="9" t="s">
         <v>106</v>
       </c>
-      <c r="G56" s="9" t="s">
+      <c r="G56" s="9"/>
+      <c r="H56" s="9" t="s">
         <v>449</v>
       </c>
-      <c r="H56" s="9" t="s">
+      <c r="I56" s="9" t="s">
         <v>443</v>
       </c>
-      <c r="I56" s="9" t="s">
+      <c r="J56" s="9" t="s">
         <v>325</v>
       </c>
-      <c r="J56" s="12" t="s">
+      <c r="K56" s="12" t="s">
         <v>106</v>
       </c>
-      <c r="K56" s="12" t="s">
+      <c r="L56" s="12" t="s">
         <v>267</v>
       </c>
-      <c r="L56" s="11" t="s">
-        <v>188</v>
-      </c>
       <c r="M56" s="11" t="s">
-        <v>189</v>
-      </c>
-      <c r="N56" s="4" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="57" spans="1:14" ht="15">
+        <v>188</v>
+      </c>
+      <c r="N56" s="11" t="s">
+        <v>189</v>
+      </c>
+      <c r="O56" s="4" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="57" spans="1:15" ht="15">
       <c r="A57" s="8">
         <v>45982</v>
       </c>
@@ -4390,154 +4561,199 @@
       <c r="F57" s="9" t="s">
         <v>106</v>
       </c>
-      <c r="G57" s="9" t="s">
+      <c r="G57" s="9"/>
+      <c r="H57" s="9" t="s">
         <v>449</v>
       </c>
-      <c r="H57" s="9" t="s">
+      <c r="I57" s="9" t="s">
         <v>445</v>
       </c>
-      <c r="I57" s="9" t="s">
+      <c r="J57" s="9" t="s">
         <v>325</v>
       </c>
-      <c r="J57" s="12" t="s">
+      <c r="K57" s="12" t="s">
         <v>106</v>
       </c>
-      <c r="K57" s="12" t="s">
+      <c r="L57" s="12" t="s">
         <v>267</v>
       </c>
-      <c r="L57" s="11" t="s">
-        <v>188</v>
-      </c>
       <c r="M57" s="11" t="s">
-        <v>189</v>
-      </c>
-      <c r="N57" s="4" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="58" spans="1:14" ht="14.25">
+        <v>188</v>
+      </c>
+      <c r="N57" s="11" t="s">
+        <v>189</v>
+      </c>
+      <c r="O57" s="4" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="58" spans="1:15" ht="14.25">
       <c r="E58" s="19" t="s">
         <v>441</v>
       </c>
       <c r="F58" s="20" t="s">
         <v>452</v>
       </c>
-      <c r="G58" t="s">
+      <c r="G58" s="27"/>
+      <c r="H58" t="s">
         <v>452</v>
+      </c>
+    </row>
+    <row r="61" spans="1:15">
+      <c r="A61" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="62" spans="1:15">
+      <c r="A62" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="63" spans="1:15">
+      <c r="A63" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="64" spans="1:15">
+      <c r="A64" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2">
+      <c r="A65" t="s">
+        <v>460</v>
+      </c>
+      <c r="B65" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2">
+      <c r="A66" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2">
+      <c r="A67" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2">
+      <c r="A68" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2">
+      <c r="A69" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2">
+      <c r="A70" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2">
+      <c r="A71" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2">
+      <c r="A72" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2">
+      <c r="A73" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2">
+      <c r="A74" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2">
+      <c r="A75" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2">
+      <c r="A76" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2">
+      <c r="A77" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2">
+      <c r="A78" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2">
+      <c r="A79" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2">
+      <c r="A80" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1">
+      <c r="A81" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1">
+      <c r="A82" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1">
+      <c r="A83" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1">
+      <c r="A84" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1">
+      <c r="A85" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1">
+      <c r="A86" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1">
+      <c r="A87" t="s">
+        <v>350</v>
       </c>
     </row>
   </sheetData>
   <protectedRanges>
-    <protectedRange sqref="H33" name="Database"/>
+    <protectedRange sqref="I33" name="Database"/>
   </protectedRanges>
-  <autoFilter ref="A8:N58" xr:uid="{F368BCE2-BE99-4B2E-A17A-1E5FAB5A74C3}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A9:N58">
-      <sortCondition ref="F8:F58"/>
-    </sortState>
-  </autoFilter>
-  <conditionalFormatting sqref="E53:E58 A8:N52">
-    <cfRule type="expression" dxfId="30" priority="38">
+  <conditionalFormatting sqref="A8:O57">
+    <cfRule type="expression" dxfId="34" priority="21">
       <formula>$A8=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N53:N57 B53:B57 E53:H57 E58:F58">
-    <cfRule type="expression" dxfId="29" priority="20">
+  <conditionalFormatting sqref="E53:E58">
+    <cfRule type="expression" dxfId="33" priority="58">
       <formula>$A53=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J53:M53">
-    <cfRule type="expression" dxfId="28" priority="19">
-      <formula>$A53=TODAY()</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J54:M57">
-    <cfRule type="expression" dxfId="27" priority="18">
-      <formula>$A54=TODAY()</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I53">
-    <cfRule type="expression" dxfId="26" priority="17">
-      <formula>$A53=TODAY()</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I54">
-    <cfRule type="expression" dxfId="25" priority="16">
-      <formula>$A54=TODAY()</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I55">
-    <cfRule type="expression" dxfId="24" priority="15">
-      <formula>$A55=TODAY()</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I56">
-    <cfRule type="expression" dxfId="23" priority="14">
-      <formula>$A56=TODAY()</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I57">
-    <cfRule type="expression" dxfId="22" priority="13">
-      <formula>$A57=TODAY()</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A53">
-    <cfRule type="expression" dxfId="21" priority="12">
-      <formula>$A53=TODAY()</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A54:A57">
-    <cfRule type="expression" dxfId="20" priority="11">
-      <formula>$A54=TODAY()</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C53">
-    <cfRule type="expression" dxfId="19" priority="10">
-      <formula>$A53=TODAY()</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C54">
-    <cfRule type="expression" dxfId="18" priority="9">
-      <formula>$A54=TODAY()</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C55">
-    <cfRule type="expression" dxfId="17" priority="8">
-      <formula>$A55=TODAY()</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C56">
-    <cfRule type="expression" dxfId="16" priority="7">
-      <formula>$A56=TODAY()</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C57">
-    <cfRule type="expression" dxfId="15" priority="6">
-      <formula>$A57=TODAY()</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D53">
-    <cfRule type="expression" dxfId="14" priority="5">
-      <formula>$A53=TODAY()</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D54">
-    <cfRule type="expression" dxfId="13" priority="4">
-      <formula>$A54=TODAY()</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D55">
-    <cfRule type="expression" dxfId="12" priority="3">
-      <formula>$A55=TODAY()</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D56">
-    <cfRule type="expression" dxfId="11" priority="2">
-      <formula>$A56=TODAY()</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D57">
-    <cfRule type="expression" dxfId="10" priority="1">
-      <formula>$A57=TODAY()</formula>
+  <conditionalFormatting sqref="E58:G58">
+    <cfRule type="expression" dxfId="32" priority="40">
+      <formula>$A58=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8839,48 +9055,48 @@
   <protectedRanges>
     <protectedRange sqref="H78" name="Database_1_1"/>
   </protectedRanges>
-  <conditionalFormatting sqref="N2:N97 A2:E97 G2:H97">
-    <cfRule type="expression" dxfId="9" priority="10">
+  <conditionalFormatting sqref="A2:H97">
+    <cfRule type="expression" dxfId="31" priority="1">
       <formula>$A2=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="A1:N1">
+    <cfRule type="expression" dxfId="30" priority="2">
+      <formula>$A1=TODAY()</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="I2:I70">
-    <cfRule type="expression" dxfId="8" priority="9">
+    <cfRule type="expression" dxfId="29" priority="9">
       <formula>$A2=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I71:K71">
-    <cfRule type="expression" dxfId="7" priority="4">
+    <cfRule type="expression" dxfId="28" priority="4">
       <formula>$A71=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I72:M97">
-    <cfRule type="expression" dxfId="6" priority="3">
+    <cfRule type="expression" dxfId="27" priority="3">
       <formula>$A72=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J27:K70">
-    <cfRule type="expression" dxfId="5" priority="5">
+    <cfRule type="expression" dxfId="26" priority="5">
       <formula>$A27=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J2:M26">
-    <cfRule type="expression" dxfId="4" priority="8">
+    <cfRule type="expression" dxfId="25" priority="8">
       <formula>$A2=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L27:M71">
-    <cfRule type="expression" dxfId="3" priority="6">
+    <cfRule type="expression" dxfId="24" priority="6">
       <formula>$A27=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:N1">
-    <cfRule type="expression" dxfId="2" priority="2">
-      <formula>$A1=TODAY()</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F2:F97">
-    <cfRule type="expression" dxfId="1" priority="1">
+  <conditionalFormatting sqref="N2:N97">
+    <cfRule type="expression" dxfId="23" priority="10">
       <formula>$A2=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10173,7 +10389,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C55">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="22" priority="1">
       <formula>$A55=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
20260210 EUEPR GHCPR + EDWPE partially
</commit_message>
<xml_diff>
--- a/GUI + Reviews/New indices list.xlsx
+++ b/GUI + Reviews/New indices list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://euronext-my.sharepoint.com/personal/csonneveld_euronext_com/Documents/Documents/Projects/GUI + Reviews/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="534" documentId="8_{676A6875-F432-47B7-9717-3084B8EAD88C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{63B0EC59-0E98-4FE7-BE30-96EAE5F7C1A8}"/>
+  <xr:revisionPtr revIDLastSave="546" documentId="8_{676A6875-F432-47B7-9717-3084B8EAD88C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4328702A-4DED-4FB4-8DD5-AF6F7E63812D}"/>
   <bookViews>
     <workbookView xWindow="-29115" yWindow="-16005" windowWidth="29040" windowHeight="15720" xr2:uid="{470E612D-E4A8-42B4-A972-1027153868F9}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1965" uniqueCount="483">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1977" uniqueCount="487">
   <si>
     <t>EEUS</t>
   </si>
@@ -1490,6 +1490,18 @@
   </si>
   <si>
     <t>IWUTP</t>
+  </si>
+  <si>
+    <t>Even nakijken verkeerde Naming</t>
+  </si>
+  <si>
+    <t>prio</t>
+  </si>
+  <si>
+    <t>Prio</t>
+  </si>
+  <si>
+    <t>Work in Progress</t>
   </si>
 </sst>
 </file>
@@ -2327,10 +2339,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F368BCE2-BE99-4B2E-A17A-1E5FAB5A74C3}">
-  <dimension ref="A1:O90"/>
+  <dimension ref="A1:O93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A61" sqref="A61"/>
+    <sheetView tabSelected="1" topLeftCell="A50" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D82" sqref="D82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -3328,7 +3340,9 @@
       <c r="F29" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="G29" s="9"/>
+      <c r="G29" s="9" t="s">
+        <v>456</v>
+      </c>
       <c r="H29" s="9"/>
       <c r="I29" s="9" t="s">
         <v>363</v>
@@ -3371,7 +3385,9 @@
       <c r="F30" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="G30" s="9"/>
+      <c r="G30" s="9" t="s">
+        <v>456</v>
+      </c>
       <c r="H30" s="9"/>
       <c r="I30" s="9" t="s">
         <v>376</v>
@@ -3589,7 +3605,9 @@
         <v>115</v>
       </c>
       <c r="G35" s="9"/>
-      <c r="H35" s="9"/>
+      <c r="H35" s="9" t="s">
+        <v>485</v>
+      </c>
       <c r="I35" s="9" t="s">
         <v>407</v>
       </c>
@@ -3632,7 +3650,9 @@
         <v>115</v>
       </c>
       <c r="G36" s="9"/>
-      <c r="H36" s="9"/>
+      <c r="H36" s="9" t="s">
+        <v>485</v>
+      </c>
       <c r="I36" s="4" t="s">
         <v>409</v>
       </c>
@@ -3675,7 +3695,9 @@
         <v>115</v>
       </c>
       <c r="G37" s="9"/>
-      <c r="H37" s="9"/>
+      <c r="H37" s="9" t="s">
+        <v>485</v>
+      </c>
       <c r="I37" s="9" t="s">
         <v>411</v>
       </c>
@@ -3718,7 +3740,9 @@
         <v>115</v>
       </c>
       <c r="G38" s="9"/>
-      <c r="H38" s="9"/>
+      <c r="H38" s="9" t="s">
+        <v>485</v>
+      </c>
       <c r="I38" s="9" t="s">
         <v>413</v>
       </c>
@@ -3761,7 +3785,9 @@
         <v>115</v>
       </c>
       <c r="G39" s="9"/>
-      <c r="H39" s="9"/>
+      <c r="H39" s="9" t="s">
+        <v>484</v>
+      </c>
       <c r="I39" s="9" t="s">
         <v>415</v>
       </c>
@@ -4605,6 +4631,9 @@
       <c r="A62" t="s">
         <v>457</v>
       </c>
+      <c r="B62" t="s">
+        <v>483</v>
+      </c>
     </row>
     <row r="63" spans="1:15">
       <c r="A63" t="s">
@@ -4699,54 +4728,72 @@
         <v>476</v>
       </c>
     </row>
-    <row r="81" spans="1:1">
+    <row r="81" spans="1:2">
       <c r="A81" t="s">
         <v>478</v>
       </c>
     </row>
-    <row r="82" spans="1:1">
+    <row r="82" spans="1:2">
       <c r="A82" t="s">
         <v>477</v>
       </c>
     </row>
-    <row r="83" spans="1:1">
+    <row r="83" spans="1:2">
       <c r="A83" t="s">
         <v>479</v>
       </c>
     </row>
-    <row r="84" spans="1:1">
+    <row r="84" spans="1:2">
       <c r="A84" t="s">
         <v>481</v>
       </c>
     </row>
-    <row r="85" spans="1:1">
+    <row r="85" spans="1:2">
       <c r="A85" t="s">
         <v>480</v>
       </c>
     </row>
-    <row r="86" spans="1:1">
+    <row r="86" spans="1:2">
       <c r="A86" t="s">
         <v>482</v>
       </c>
     </row>
-    <row r="87" spans="1:1">
+    <row r="87" spans="1:2">
       <c r="A87" t="s">
         <v>350</v>
       </c>
     </row>
-    <row r="88" spans="1:1">
+    <row r="88" spans="1:2">
       <c r="A88" t="s">
         <v>348</v>
       </c>
     </row>
-    <row r="89" spans="1:1">
+    <row r="89" spans="1:2">
       <c r="A89" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="90" spans="1:1">
+    <row r="90" spans="1:2">
       <c r="A90" t="s">
         <v>359</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2">
+      <c r="A91" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2">
+      <c r="A92" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2">
+      <c r="A93" t="s">
+        <v>414</v>
+      </c>
+      <c r="B93" t="s">
+        <v>486</v>
       </c>
     </row>
   </sheetData>

</xml_diff>